<commit_message>
preliminary beamforming is working
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -140,9 +140,6 @@
     <t>atten-&gt;write atten values</t>
   </si>
   <si>
-    <t>takes values 1-&gt;8 for channels 0-&gt;7 (reg value of 0 does nothing)</t>
-  </si>
-  <si>
     <t>chan 0-&gt;bits(7 downto 0); chan 1-&gt; bits(15 downto 8); chan2-&gt;bits(23 downto 16)</t>
   </si>
   <si>
@@ -159,6 +156,15 @@
   </si>
   <si>
     <t>adc-&gt;dclk_rst pulse</t>
+  </si>
+  <si>
+    <t>takes values 1-&gt;num_beams for wfms chans 0-&gt;7  and beams (reg value of 0 does nothing)</t>
+  </si>
+  <si>
+    <t>rdout-&gt;ram select</t>
+  </si>
+  <si>
+    <t>LSB-&gt;wfm ram; LSB+1-&gt;beam ram</t>
   </si>
 </sst>
 </file>
@@ -204,9 +210,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,74 +495,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>42788</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -904,7 +910,7 @@
         <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
@@ -916,10 +922,10 @@
         <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D58" t="s">
         <v>8</v>
@@ -931,10 +937,10 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
         <v>42</v>
-      </c>
-      <c r="C59" t="s">
-        <v>43</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -967,7 +973,7 @@
         <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C62" t="s">
         <v>20</v>
@@ -1048,7 +1054,7 @@
         <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
@@ -1058,6 +1064,15 @@
       <c r="A73">
         <f t="shared" si="0"/>
         <v>66</v>
+      </c>
+      <c r="B73" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working towards MCU interface
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -47,9 +47,6 @@
     <t>reset register</t>
   </si>
   <si>
-    <t>power-up value</t>
-  </si>
-  <si>
     <t>0x000000</t>
   </si>
   <si>
@@ -165,6 +162,39 @@
   </si>
   <si>
     <t>LSB-&gt;wfm ram; LSB+1-&gt;beam ram</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>adc-&gt;serdes delay ADC0</t>
+  </si>
+  <si>
+    <t>adc-&gt;serdes delay ADC1</t>
+  </si>
+  <si>
+    <t>adc-&gt;serdes delay ADC2</t>
+  </si>
+  <si>
+    <t>adc-&gt;serdes delay ADC3</t>
+  </si>
+  <si>
+    <t>lower 4 bits set delay</t>
+  </si>
+  <si>
+    <t>power-up default value</t>
+  </si>
+  <si>
+    <t>clock select</t>
+  </si>
+  <si>
+    <t>master 100 MHz clock select: local oscillator (==1) or external LVDS input (==0)</t>
+  </si>
+  <si>
+    <t>lower bit only</t>
+  </si>
+  <si>
+    <t>not really useful -- data alignment done using registers 56 to 59. Pulse this in order to get ADCs within one deserialized clock cycle</t>
   </si>
 </sst>
 </file>
@@ -208,11 +238,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,52 +535,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="80.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" style="5" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42788</v>
+        <v>42870</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,9 +602,9 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -569,13 +612,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -583,10 +626,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -595,10 +638,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -607,10 +650,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -619,10 +662,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,10 +674,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -661,97 +704,109 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -853,145 +908,166 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B60" t="s">
         <v>36</v>
       </c>
-      <c r="C57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" si="0"/>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B63" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" t="s">
         <v>51</v>
       </c>
-      <c r="B58" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" t="s">
-        <v>39</v>
-      </c>
-      <c r="D58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B62" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>57</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -999,12 +1075,30 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
+      <c r="B65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
+      <c r="B66" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
@@ -1036,13 +1130,13 @@
         <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,13 +1145,13 @@
         <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,13 +1160,13 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" t="s">
         <v>45</v>
       </c>
-      <c r="C73" t="s">
-        <v>46</v>
-      </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,10 +1175,10 @@
         <v>67</v>
       </c>
       <c r="B74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" t="s">
         <v>15</v>
-      </c>
-      <c r="D74" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,10 +1187,10 @@
         <v>68</v>
       </c>
       <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
         <v>17</v>
-      </c>
-      <c r="D75" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1205,13 @@
         <v>70</v>
       </c>
       <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
         <v>19</v>
       </c>
-      <c r="C77" t="s">
-        <v>20</v>
-      </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,13 +1220,13 @@
         <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1141,13 +1235,13 @@
         <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,10 +1256,10 @@
         <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,10 +1268,10 @@
         <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,10 +1589,10 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working towards MCU integration
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -195,6 +196,12 @@
   </si>
   <si>
     <t>not really useful -- data alignment done using registers 56 to 59. Pulse this in order to get ADCs within one deserialized clock cycle</t>
+  </si>
+  <si>
+    <t>rdout-&gt;ram address</t>
+  </si>
+  <si>
+    <t>current RAM address pointer</t>
   </si>
 </sst>
 </file>
@@ -243,7 +250,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -253,6 +259,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,34 +552,34 @@
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="80.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="73.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -582,7 +589,7 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -604,7 +611,7 @@
       <c r="D6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -754,7 +761,7 @@
       <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1036,7 +1043,7 @@
       <c r="D62" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1197,6 +1204,12 @@
       <c r="A76">
         <f t="shared" si="1"/>
         <v>69</v>
+      </c>
+      <c r="B76" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
compiled MCU spi_slave interface
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -159,12 +159,6 @@
     <t>takes values 1-&gt;num_beams for wfms chans 0-&gt;7  and beams (reg value of 0 does nothing)</t>
   </si>
   <si>
-    <t>rdout-&gt;ram select</t>
-  </si>
-  <si>
-    <t>LSB-&gt;wfm ram; LSB+1-&gt;beam ram</t>
-  </si>
-  <si>
     <t>NOTE</t>
   </si>
   <si>
@@ -202,13 +196,31 @@
   </si>
   <si>
     <t>current RAM address pointer</t>
+  </si>
+  <si>
+    <t>USB readout only</t>
+  </si>
+  <si>
+    <t>LSB-&gt;wfm ram; LSB+1-&gt;beam ram…all 0's for register read</t>
+  </si>
+  <si>
+    <t>rdout-&gt;readout type</t>
+  </si>
+  <si>
+    <t>for MCU interface, write this register to initiate readout</t>
+  </si>
+  <si>
+    <t>rdout-&gt;data chunk</t>
+  </si>
+  <si>
+    <t>spi slave is 32 bits, RAM width is 128 bits. Specify which 32 bit chunk of RAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +232,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,10 +264,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -260,6 +280,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,34 +577,34 @@
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="80.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="73.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" style="5" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -589,8 +614,8 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>46</v>
+      <c r="E4" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -609,9 +634,9 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -753,16 +778,16 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>55</v>
+      <c r="E23" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1043,8 +1068,8 @@
       <c r="D62" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>56</v>
+      <c r="E62" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,10 +1078,10 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
@@ -1068,70 +1093,70 @@
         <v>57</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1146,7 +1171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1161,58 +1186,67 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
         <f t="shared" ref="A74:A134" si="1">1+A73</f>
         <v>67</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="E74" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="E75" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B76" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1226,23 +1260,29 @@
       <c r="D77" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="E77" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1257,115 +1297,130 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="B80" t="s">
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
+      <c r="E81" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>89</v>

</xml_diff>

<commit_message>
working fast ref pulse output for ADC alignment
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -126,12 +126,6 @@
     <t>0x000001</t>
   </si>
   <si>
-    <t>status_1</t>
-  </si>
-  <si>
-    <t>status_2</t>
-  </si>
-  <si>
     <t>atten-&gt;chan0,1,2</t>
   </si>
   <si>
@@ -214,6 +208,45 @@
   </si>
   <si>
     <t>spi slave is 32 bits, RAM width is 128 bits. Specify which 32 bit chunk of RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>RF switch select</t>
+  </si>
+  <si>
+    <t>RF pulse enable</t>
+  </si>
+  <si>
+    <t>pick off debug header?</t>
+  </si>
+  <si>
+    <t>use trig_out aux SMA</t>
+  </si>
+  <si>
+    <t>toggle input switch between signal and ref pulse (LSB=1 switch to cal pulse input)</t>
+  </si>
+  <si>
+    <t>toggle FPGA-generated fast pulse (LSB=1 enable, LSB=0 disable)</t>
+  </si>
+  <si>
+    <t>chip_id(low)</t>
+  </si>
+  <si>
+    <t>chip_id(mid)</t>
+  </si>
+  <si>
+    <t>chip_id(high)</t>
+  </si>
+  <si>
+    <t>mid 24 bits</t>
+  </si>
+  <si>
+    <t>chip is 64 bits: lower 24 bits</t>
+  </si>
+  <si>
+    <t>high 16 bits</t>
   </si>
 </sst>
 </file>
@@ -567,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +648,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -634,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -694,11 +727,14 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
+      <c r="E11" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -706,17 +742,29 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
+      <c r="E12" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -778,16 +826,16 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,100 +892,112 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,6 +1005,18 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -994,10 +1066,10 @@
         <v>50</v>
       </c>
       <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
         <v>35</v>
-      </c>
-      <c r="C57" t="s">
-        <v>37</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -1009,10 +1081,10 @@
         <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -1024,10 +1096,10 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -1039,7 +1111,7 @@
         <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s">
         <v>19</v>
@@ -1060,7 +1132,7 @@
         <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
         <v>19</v>
@@ -1069,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,10 +1150,10 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C63" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
@@ -1093,10 +1165,10 @@
         <v>57</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>7</v>
@@ -1108,10 +1180,10 @@
         <v>58</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>7</v>
@@ -1123,10 +1195,10 @@
         <v>59</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
@@ -1180,7 +1252,7 @@
         <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D72" t="s">
         <v>9</v>
@@ -1192,10 +1264,10 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
@@ -1213,7 +1285,7 @@
         <v>15</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1228,7 +1300,7 @@
         <v>17</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1237,10 +1309,10 @@
         <v>69</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
@@ -1261,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1279,7 +1351,7 @@
         <v>9</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,10 +1375,10 @@
         <v>73</v>
       </c>
       <c r="B80" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>9</v>
@@ -1324,7 +1396,7 @@
         <v>22</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1339,7 +1411,7 @@
         <v>25</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,6 +1436,9 @@
       <c r="A86">
         <f t="shared" si="1"/>
         <v>79</v>
+      </c>
+      <c r="C86" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working spi interface, move RF switch control to SMA control
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -213,24 +212,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>RF switch select</t>
-  </si>
-  <si>
-    <t>RF pulse enable</t>
-  </si>
-  <si>
-    <t>pick off debug header?</t>
-  </si>
-  <si>
-    <t>use trig_out aux SMA</t>
-  </si>
-  <si>
-    <t>toggle input switch between signal and ref pulse (LSB=1 switch to cal pulse input)</t>
-  </si>
-  <si>
-    <t>toggle FPGA-generated fast pulse (LSB=1 enable, LSB=0 disable)</t>
-  </si>
-  <si>
     <t>chip_id(low)</t>
   </si>
   <si>
@@ -247,13 +228,22 @@
   </si>
   <si>
     <t>high 16 bits</t>
+  </si>
+  <si>
+    <t>cal pulser board</t>
+  </si>
+  <si>
+    <t>toggle FPGA-generated fast pulse w/ LSB, toggle RF switch with LSB+1</t>
+  </si>
+  <si>
+    <t>use trig_out aux SMA for pulse, trig_in SMA (inout) fo switch select</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +262,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -312,12 +308,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,28 +612,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -727,13 +724,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -742,13 +739,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -757,13 +754,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,112 +889,100 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>41</v>
-      </c>
-      <c r="B48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1006,16 +991,16 @@
         <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,85 +1258,85 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="10">
+    <row r="74" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
         <f t="shared" ref="A74:A134" si="1">1+A73</f>
         <v>67</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="10" t="s">
+      <c r="D74" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="E74" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="10">
+    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="10" t="s">
+      <c r="D75" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="E75" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+      <c r="A76" s="8">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="77" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="10">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,33 +1369,33 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10">
+    <row r="81" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="9">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="10" t="s">
+      <c r="D81" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="E81" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="10">
+    <row r="82" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D82" s="10" t="s">
+      <c r="D82" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E82" s="10" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add ADC pd register
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>use trig_out aux SMA for pulse, trig_in SMA (inout) fo switch select</t>
+  </si>
+  <si>
+    <t>adc-&gt;powerdown (pd)</t>
+  </si>
+  <si>
+    <t>lower 4 bits set PD (I+Q channel, ADCs 0-&gt;3)</t>
   </si>
 </sst>
 </file>
@@ -293,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +314,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -597,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,28 +619,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,205 +788,206 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C39" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D39" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1194,6 +1202,15 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -1258,81 +1275,81 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
         <f t="shared" ref="A74:A134" si="1">1+A73</f>
         <v>67</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D74" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="E74" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
+    <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="E75" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+      <c r="A76" s="9">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+    <row r="77" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="10">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D77" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E77" s="10" t="s">
+      <c r="E77" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
+    <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E78" s="5" t="s">
@@ -1369,33 +1386,33 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+    <row r="81" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="E81" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+    <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D82" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="E82" s="11" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to data readout, given a trigger
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -324,13 +324,13 @@
     <t>trigger mask</t>
   </si>
   <si>
-    <t>beam mask in trigger</t>
-  </si>
-  <si>
     <t>0xFFFFFF</t>
   </si>
   <si>
     <t>set beam bit to 0 to mask</t>
+  </si>
+  <si>
+    <t>beam mask in trigger [LSB-&gt;(num_beams-1)]</t>
   </si>
 </sst>
 </file>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,13 +1560,13 @@
         <v>94</v>
       </c>
       <c r="C87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" t="s">
         <v>95</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add pre trig window, update doc
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -51,9 +51,6 @@
     <t>0x000000</t>
   </si>
   <si>
-    <t>current 32 bit register space: 8 bit address, 24 bit data (128 24-bit registers)</t>
-  </si>
-  <si>
     <t>x000000</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
   </si>
   <si>
     <t>rdout-&gt;readout type</t>
-  </si>
-  <si>
-    <t>for MCU interface, write this register to initiate readout</t>
   </si>
   <si>
     <t>rdout-&gt;data chunk</t>
@@ -331,6 +325,27 @@
   </si>
   <si>
     <t>beam mask in trigger [LSB-&gt;(num_beams-1)]</t>
+  </si>
+  <si>
+    <t>for BBB interface, write this register to initiate readout</t>
+  </si>
+  <si>
+    <t>rdout-&gt;pretrigger window</t>
+  </si>
+  <si>
+    <t>lower three bits used, set value to 0 thru 5. Pretrig window set to value*8*10.66ns</t>
+  </si>
+  <si>
+    <t>read_only - board DNA (FPGA silicon-specific ID)</t>
+  </si>
+  <si>
+    <t>start thresholds off at max</t>
+  </si>
+  <si>
+    <t>nothing defined here yet</t>
+  </si>
+  <si>
+    <t>current 32 bit register space: 8 bit address + 24 bit data (i.e. 128 24-bit registers)</t>
   </si>
 </sst>
 </file>
@@ -700,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,14 +756,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42870</v>
+        <v>42917</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +782,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -777,13 +792,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -791,10 +806,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -803,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,10 +830,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -827,13 +845,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -842,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -857,13 +875,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
+        <v>60</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -871,60 +889,90 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="C14" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="C15" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="C16" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="C17" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="C18" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="C19" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="C20" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="C21" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="C22" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="C23" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,90 +980,135 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
+      <c r="C24" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+      <c r="C25" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="C26" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="C27" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="C28" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
+      <c r="C29" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
+      <c r="C30" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
+      <c r="C31" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="C32" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
+      <c r="C33" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
+      <c r="C34" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="C35" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
+      <c r="C36" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="C37" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
+      <c r="C38" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -1023,16 +1116,16 @@
         <v>32</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="D39" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1095,16 +1188,16 @@
         <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1143,10 +1236,10 @@
         <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -1164,10 +1257,10 @@
         <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -1179,10 +1272,10 @@
         <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -1194,10 +1287,10 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" t="s">
         <v>38</v>
-      </c>
-      <c r="C59" t="s">
-        <v>39</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -1209,10 +1302,10 @@
         <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -1230,16 +1323,16 @@
         <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,10 +1341,10 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
@@ -1263,10 +1356,10 @@
         <v>57</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>7</v>
@@ -1278,10 +1371,10 @@
         <v>58</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>7</v>
@@ -1293,10 +1386,10 @@
         <v>59</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
@@ -1308,10 +1401,10 @@
         <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -1341,13 +1434,13 @@
         <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,13 +1449,13 @@
         <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1371,16 +1464,16 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1389,13 +1482,13 @@
         <v>67</v>
       </c>
       <c r="B74" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="E74" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1404,13 +1497,13 @@
         <v>68</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="E75" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,13 +1512,13 @@
         <v>69</v>
       </c>
       <c r="B76" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1434,16 +1527,16 @@
         <v>70</v>
       </c>
       <c r="B77" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C77" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="D77" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1452,16 +1545,16 @@
         <v>71</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,13 +1563,13 @@
         <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,13 +1578,13 @@
         <v>73</v>
       </c>
       <c r="B80" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C80" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1500,13 +1593,13 @@
         <v>74</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1515,13 +1608,13 @@
         <v>75</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1529,6 +1622,15 @@
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>98</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -1548,7 +1650,7 @@
         <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,16 +1659,16 @@
         <v>80</v>
       </c>
       <c r="B87" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" t="s">
+        <v>93</v>
+      </c>
+      <c r="E87" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="C87" t="s">
-        <v>97</v>
-      </c>
-      <c r="D87" t="s">
-        <v>95</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,13 +1708,16 @@
         <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1621,13 +1726,13 @@
         <v>87</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,13 +1741,13 @@
         <v>88</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,13 +1756,13 @@
         <v>89</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1666,13 +1771,13 @@
         <v>90</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,13 +1786,13 @@
         <v>91</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,13 +1801,13 @@
         <v>92</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1711,13 +1816,13 @@
         <v>93</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1726,13 +1831,13 @@
         <v>94</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,13 +1846,13 @@
         <v>95</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,13 +1861,13 @@
         <v>96</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,13 +1876,13 @@
         <v>97</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,13 +1891,13 @@
         <v>98</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,13 +1906,13 @@
         <v>99</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1816,13 +1921,13 @@
         <v>100</v>
       </c>
       <c r="B107" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D107" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1831,13 +1936,13 @@
         <v>101</v>
       </c>
       <c r="B108" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C108" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="D108" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,10 +2104,10 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D134" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix timing issues in adc controller
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -175,9 +174,6 @@
   </si>
   <si>
     <t>master 100 MHz clock select: local oscillator (==1) or external LVDS input (==0)</t>
-  </si>
-  <si>
-    <t>not really useful -- data alignment done using registers 56 to 59. Pulse this in order to get ADCs within one deserialized clock cycle</t>
   </si>
   <si>
     <t>rdout-&gt;ram address</t>
@@ -736,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +777,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>41</v>
@@ -857,7 +853,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,13 +862,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -881,13 +877,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,13 +892,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -911,13 +907,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,7 +1148,7 @@
         <v>31</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1215,16 +1211,16 @@
         <v>42</v>
       </c>
       <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
         <v>64</v>
-      </c>
-      <c r="C49" t="s">
-        <v>65</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,10 +1259,10 @@
         <v>48</v>
       </c>
       <c r="B55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" t="s">
         <v>70</v>
-      </c>
-      <c r="C55" t="s">
-        <v>71</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -1344,7 +1340,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1353,14 +1349,11 @@
         <v>39</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -1428,10 +1421,10 @@
         <v>60</v>
       </c>
       <c r="B67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" t="s">
         <v>67</v>
-      </c>
-      <c r="C67" t="s">
-        <v>68</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -1491,16 +1484,16 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D73" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1515,7 +1508,7 @@
         <v>14</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1530,7 +1523,7 @@
         <v>16</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,10 +1532,10 @@
         <v>69</v>
       </c>
       <c r="B76" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -1563,7 +1556,7 @@
         <v>8</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1581,7 +1574,7 @@
         <v>8</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1605,10 +1598,10 @@
         <v>73</v>
       </c>
       <c r="B80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" t="s">
         <v>55</v>
-      </c>
-      <c r="C80" t="s">
-        <v>56</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>8</v>
@@ -1626,7 +1619,7 @@
         <v>21</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1641,7 +1634,7 @@
         <v>24</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,10 +1643,10 @@
         <v>76</v>
       </c>
       <c r="B83" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" t="s">
         <v>97</v>
-      </c>
-      <c r="C83" t="s">
-        <v>98</v>
       </c>
       <c r="D83" t="s">
         <v>8</v>
@@ -1665,10 +1658,10 @@
         <v>77</v>
       </c>
       <c r="B84" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" t="s">
         <v>103</v>
-      </c>
-      <c r="C84" t="s">
-        <v>104</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>
@@ -1680,16 +1673,16 @@
         <v>78</v>
       </c>
       <c r="B85" t="s">
+        <v>104</v>
+      </c>
+      <c r="C85" t="s">
         <v>105</v>
-      </c>
-      <c r="C85" t="s">
-        <v>106</v>
       </c>
       <c r="D85" t="s">
         <v>8</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,7 +1691,7 @@
         <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1707,16 +1700,16 @@
         <v>80</v>
       </c>
       <c r="B87" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" t="s">
         <v>92</v>
       </c>
-      <c r="C87" t="s">
-        <v>95</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,16 +1749,16 @@
         <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1774,13 +1767,13 @@
         <v>87</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -1789,13 +1782,13 @@
         <v>88</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,13 +1797,13 @@
         <v>89</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,13 +1812,13 @@
         <v>90</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1834,13 +1827,13 @@
         <v>91</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,13 +1842,13 @@
         <v>92</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,13 +1857,13 @@
         <v>93</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1879,13 +1872,13 @@
         <v>94</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1894,13 +1887,13 @@
         <v>95</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,13 +1902,13 @@
         <v>96</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,13 +1917,13 @@
         <v>97</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,13 +1932,13 @@
         <v>98</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,13 +1947,13 @@
         <v>99</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,13 +1962,13 @@
         <v>100</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,13 +1977,13 @@
         <v>101</v>
       </c>
       <c r="B108" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D108" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add event metadata, update doc register map
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="131">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -378,6 +379,57 @@
   </si>
   <si>
     <t>scaler_to_read</t>
+  </si>
+  <si>
+    <t>write LSB</t>
+  </si>
+  <si>
+    <t>read_only - event meta data</t>
+  </si>
+  <si>
+    <t>reset event counter/timestamp</t>
+  </si>
+  <si>
+    <t>metadata-&gt;event counter low</t>
+  </si>
+  <si>
+    <t>metadata-&gt;event counter high</t>
+  </si>
+  <si>
+    <t>metadata-&gt;trig counter low</t>
+  </si>
+  <si>
+    <t>metadata-&gt;trig counter high</t>
+  </si>
+  <si>
+    <t>metadata-&gt;trig timestamp low</t>
+  </si>
+  <si>
+    <t>metadata-&gt;trig timestamp high</t>
+  </si>
+  <si>
+    <t>metadata-&gt;deadtime counter</t>
+  </si>
+  <si>
+    <t>deadtime counter refreshed every second</t>
+  </si>
+  <si>
+    <t>note: metadata assigned to these registers once event buffer set in register 78</t>
+  </si>
+  <si>
+    <t>metadata-&gt;(buffer, trig_type, trig_lastbeam)</t>
+  </si>
+  <si>
+    <t>metadata-&gt;(channel, beam masks)</t>
+  </si>
+  <si>
+    <t>metadata-&gt;unassigned</t>
+  </si>
+  <si>
+    <t>bits 23-22 : event buffer ; bits16-15: trig type ; bits 14-0: last beam trigger</t>
+  </si>
+  <si>
+    <t>bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
   </si>
 </sst>
 </file>
@@ -441,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -464,6 +516,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -747,14 +800,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
     <col min="3" max="3" width="80.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="73.5703125" style="5" customWidth="1"/>
@@ -762,28 +815,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -946,98 +999,169 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
       <c r="C17" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1046,7 +1170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1055,7 +1179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1064,7 +1188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1073,7 +1197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1082,7 +1206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2167,6 +2291,15 @@
       <c r="A133">
         <f t="shared" si="1"/>
         <v>126</v>
+      </c>
+      <c r="B133" t="s">
+        <v>116</v>
+      </c>
+      <c r="C133" t="s">
+        <v>114</v>
+      </c>
+      <c r="D133" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add power sumto metadata, tick version to 1.0
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -54,9 +54,6 @@
     <t>x000000</t>
   </si>
   <si>
-    <t>LSB-&gt;global reset</t>
-  </si>
-  <si>
     <t xml:space="preserve">LSB-&gt;force trig </t>
   </si>
   <si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>mid 24 bits</t>
-  </si>
-  <si>
-    <t>chip is 64 bits: lower 24 bits</t>
   </si>
   <si>
     <t>high 16 bits</t>
@@ -309,9 +303,6 @@
     <t>trigger mask</t>
   </si>
   <si>
-    <t>0xFFFFFF</t>
-  </si>
-  <si>
     <t>set beam bit to 0 to mask</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>read_only - board DNA (FPGA silicon-specific ID)</t>
   </si>
   <si>
-    <t>start thresholds off at max</t>
-  </si>
-  <si>
     <t>current 32 bit register space: 8 bit address + 24 bit data (i.e. 128 24-bit registers)</t>
   </si>
   <si>
@@ -348,9 +336,6 @@
     <t>4 buffers</t>
   </si>
   <si>
-    <t>0=1st buffer, and so on</t>
-  </si>
-  <si>
     <t>status reg-&gt; data manager</t>
   </si>
   <si>
@@ -417,26 +402,98 @@
     <t>note: metadata assigned to these registers once event buffer set in register 78</t>
   </si>
   <si>
-    <t>metadata-&gt;(buffer, trig_type, trig_lastbeam)</t>
-  </si>
-  <si>
     <t>metadata-&gt;(channel, beam masks)</t>
   </si>
   <si>
     <t>metadata-&gt;unassigned</t>
   </si>
   <si>
-    <t>bits 23-22 : event buffer ; bits16-15: trig type ; bits 14-0: last beam trigger</t>
-  </si>
-  <si>
     <t>bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
+  </si>
+  <si>
+    <t>bit0-&gt;global reset, bit1-&gt;reset global EXCEPT register settings, bit2-&gt;reset ADC (restart+cal cycle)</t>
+  </si>
+  <si>
+    <t>bits 23-22 : event buffer ; bit 21 : cal pulse switch ; bits 19-17 : pretrig window ; bits 16-15: trig type ; bits 14-0: last beam trigger</t>
+  </si>
+  <si>
+    <t>trigger holdoff</t>
+  </si>
+  <si>
+    <t>set trigger holdoff (this is applied to each beam, sets earliest re-trigger time in each beam)</t>
+  </si>
+  <si>
+    <t>xFFFFFF</t>
+  </si>
+  <si>
+    <t>x00000F</t>
+  </si>
+  <si>
+    <t>chip ID is 64 bits: lower 24 bits</t>
+  </si>
+  <si>
+    <t>metadata-&gt;(buffer, cal_pulse_enabletrig_type, trig_lastbeam)</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 0</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 1</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 5</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 6</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 7</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 8</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 9</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 3</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 2</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 4</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 10</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 11</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 12</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 13</t>
+  </si>
+  <si>
+    <t>metadata-&gt;power beam 14</t>
+  </si>
+  <si>
+    <t>set to: 0=1st buffer, 1=second,2=third,3=fourth</t>
+  </si>
+  <si>
+    <t>start thresholds off at max (20 bits)</t>
+  </si>
+  <si>
+    <t>lower 12 bits -&gt; max trig hold off is 4095 * 1/(93.75 MHz) = 43.7 microsecs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +529,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -493,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -518,6 +582,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,10 +910,10 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -877,13 +942,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -891,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -903,10 +968,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,10 +980,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,13 +992,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -942,13 +1007,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -957,13 +1022,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -972,13 +1037,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,7 +1052,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,7 +1061,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1005,16 +1070,16 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1088,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>7</v>
@@ -1038,10 +1103,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>7</v>
@@ -1053,10 +1118,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>7</v>
@@ -1068,10 +1133,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>7</v>
@@ -1083,10 +1148,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>7</v>
@@ -1098,34 +1163,34 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1134,16 +1199,16 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,10 +1217,10 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>7</v>
@@ -1166,8 +1231,14 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="B27" s="14" t="s">
+        <v>132</v>
+      </c>
       <c r="C27" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1175,8 +1246,14 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="B28" s="14" t="s">
+        <v>133</v>
+      </c>
       <c r="C28" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,8 +1261,14 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
+      <c r="B29" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="C29" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,8 +1276,14 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
+      <c r="B30" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="C30" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1202,8 +1291,14 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
+      <c r="B31" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="C31" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,8 +1306,14 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="B32" s="14" t="s">
+        <v>134</v>
+      </c>
       <c r="C32" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1220,8 +1321,14 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
+      <c r="B33" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="C33" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,8 +1336,14 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
+      <c r="B34" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="C34" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,8 +1351,14 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="B35" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="C35" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,8 +1366,14 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
+      <c r="B36" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="C36" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1256,8 +1381,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="B37" s="14" t="s">
+        <v>142</v>
+      </c>
       <c r="C37" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,8 +1396,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
+      <c r="B38" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="C38" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1274,17 +1411,14 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>67</v>
+      <c r="B39" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1292,12 +1426,30 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="B40" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="B41" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1335,10 +1487,10 @@
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -1350,16 +1502,16 @@
         <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,16 +1520,16 @@
         <v>42</v>
       </c>
       <c r="B49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,13 +1568,13 @@
         <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D55" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1437,10 +1589,10 @@
         <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -1452,10 +1604,10 @@
         <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -1467,10 +1619,10 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" t="s">
         <v>36</v>
-      </c>
-      <c r="C59" t="s">
-        <v>37</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -1482,10 +1634,10 @@
         <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -1503,10 +1655,10 @@
         <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -1518,10 +1670,10 @@
         <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
@@ -1533,10 +1685,10 @@
         <v>57</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>7</v>
@@ -1548,10 +1700,10 @@
         <v>58</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>7</v>
@@ -1563,10 +1715,10 @@
         <v>59</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
@@ -1578,10 +1730,10 @@
         <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -1611,10 +1763,10 @@
         <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D71" t="s">
         <v>8</v>
@@ -1626,10 +1778,10 @@
         <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
@@ -1641,16 +1793,16 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D73" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1659,13 +1811,13 @@
         <v>67</v>
       </c>
       <c r="B74" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="E74" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1674,13 +1826,13 @@
         <v>68</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D75" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="E75" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1689,10 +1841,10 @@
         <v>69</v>
       </c>
       <c r="B76" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -1704,16 +1856,16 @@
         <v>70</v>
       </c>
       <c r="B77" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1722,31 +1874,34 @@
         <v>71</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D78" s="13" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79">
+      <c r="A79" s="16">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B79" t="s">
-        <v>20</v>
-      </c>
-      <c r="C79" t="s">
-        <v>18</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="B79" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="16" t="s">
         <v>8</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1755,10 +1910,10 @@
         <v>73</v>
       </c>
       <c r="B80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C80" t="s">
         <v>53</v>
-      </c>
-      <c r="C80" t="s">
-        <v>54</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>8</v>
@@ -1770,13 +1925,13 @@
         <v>74</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1785,13 +1940,13 @@
         <v>75</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,10 +1955,10 @@
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D83" t="s">
         <v>8</v>
@@ -1815,10 +1970,10 @@
         <v>77</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C84" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>
@@ -1830,16 +1985,16 @@
         <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D85" t="s">
         <v>8</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,7 +2003,7 @@
         <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1857,16 +2012,16 @@
         <v>80</v>
       </c>
       <c r="B87" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" t="s">
         <v>89</v>
       </c>
-      <c r="C87" t="s">
-        <v>92</v>
-      </c>
       <c r="D87" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1874,6 +2029,18 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
+      <c r="B88" t="s">
+        <v>126</v>
+      </c>
+      <c r="C88" t="s">
+        <v>127</v>
+      </c>
+      <c r="D88" t="s">
+        <v>129</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -1906,16 +2073,16 @@
         <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C93" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,13 +2091,13 @@
         <v>87</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -1939,13 +2106,13 @@
         <v>88</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -1954,13 +2121,13 @@
         <v>89</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,13 +2136,13 @@
         <v>90</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,13 +2151,13 @@
         <v>91</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,13 +2166,13 @@
         <v>92</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,13 +2181,13 @@
         <v>93</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,13 +2196,13 @@
         <v>94</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,13 +2211,13 @@
         <v>95</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,13 +2226,13 @@
         <v>96</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,13 +2241,13 @@
         <v>97</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2089,13 +2256,13 @@
         <v>98</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2104,13 +2271,13 @@
         <v>99</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,13 +2286,13 @@
         <v>100</v>
       </c>
       <c r="B107" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D107" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,13 +2301,13 @@
         <v>101</v>
       </c>
       <c r="B108" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="D108" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,97 +2334,109 @@
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -2293,16 +2472,16 @@
         <v>126</v>
       </c>
       <c r="B133" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C133" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D133" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -2310,8 +2489,8 @@
       <c r="B134" t="s">
         <v>6</v>
       </c>
-      <c r="C134" t="s">
-        <v>9</v>
+      <c r="C134" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="D134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
change iface clock to 15MHz, update doc
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="151">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>bits 23-22 : event buffer ; bit 21 : cal pulse switch ; bits 19-17 : pretrig window ; bits 16-15: trig type [0=nothing,1=software,2=phased trig,3=external] ; bits 14-0: last beam trigger</t>
+  </si>
+  <si>
+    <t>lower four bits clear each of the 4 event buffers</t>
   </si>
 </sst>
 </file>
@@ -959,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E30" sqref="E29:E30"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2091,7 @@
         <v>95</v>
       </c>
       <c r="C84" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
de-reg. RAM outputs, fix SPI, debug mode w/ sigtap
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="152">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>firmware_date</t>
-  </si>
-  <si>
-    <t>pick read register</t>
   </si>
   <si>
     <t>bits 7 downto 0 select read register</t>
@@ -490,6 +487,12 @@
   </si>
   <si>
     <t>bits 3 to 0-&gt;buffer full flags; bit 8-&gt;OR of buffer full flags; bits 13 to 12-&gt;next_buffer ; bits 17 to 16-&gt; last trig type</t>
+  </si>
+  <si>
+    <t>NO FUNCTION</t>
+  </si>
+  <si>
+    <t>set read register</t>
   </si>
 </sst>
 </file>
@@ -964,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,10 +1017,10 @@
       <c r="B4" s="26"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1031,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1040,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
@@ -1054,16 +1057,7 @@
         <v>00</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1107,7 +1101,7 @@
         <v>03</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -1123,13 +1117,13 @@
         <v>04</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1142,13 +1136,13 @@
         <v>05</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,13 +1155,13 @@
         <v>06</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1180,13 +1174,13 @@
         <v>07</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1199,13 +1193,13 @@
         <v>08</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,16 +1225,16 @@
         <v>0A</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1253,10 +1247,10 @@
         <v>0B</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>7</v>
@@ -1273,10 +1267,10 @@
         <v>0C</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>7</v>
@@ -1293,10 +1287,10 @@
         <v>0D</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>7</v>
@@ -1313,10 +1307,10 @@
         <v>0E</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>7</v>
@@ -1333,10 +1327,10 @@
         <v>0F</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>7</v>
@@ -1353,16 +1347,16 @@
         <v>10</v>
       </c>
       <c r="C23" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1375,16 +1369,16 @@
         <v>11</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,16 +1391,16 @@
         <v>12</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1419,10 +1413,10 @@
         <v>13</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>7</v>
@@ -1439,7 +1433,7 @@
         <v>14</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>16</v>
@@ -1459,7 +1453,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>16</v>
@@ -1479,7 +1473,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>16</v>
@@ -1499,7 +1493,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>16</v>
@@ -1519,7 +1513,7 @@
         <v>18</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
@@ -1539,7 +1533,7 @@
         <v>19</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>16</v>
@@ -1559,7 +1553,7 @@
         <v>1A</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>16</v>
@@ -1579,7 +1573,7 @@
         <v>1B</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>16</v>
@@ -1599,7 +1593,7 @@
         <v>1C</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>16</v>
@@ -1619,7 +1613,7 @@
         <v>1D</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>16</v>
@@ -1639,7 +1633,7 @@
         <v>1E</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>16</v>
@@ -1659,7 +1653,7 @@
         <v>1F</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>16</v>
@@ -1679,7 +1673,7 @@
         <v>20</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>16</v>
@@ -1699,7 +1693,7 @@
         <v>21</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>16</v>
@@ -1719,7 +1713,7 @@
         <v>22</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>16</v>
@@ -1739,13 +1733,13 @@
         <v>23</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1758,13 +1752,13 @@
         <v>24</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,13 +1771,13 @@
         <v>25</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1796,13 +1790,13 @@
         <v>26</v>
       </c>
       <c r="C45" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" s="28" t="s">
         <v>141</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,10 +1819,10 @@
         <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1844,16 +1838,16 @@
         <v>29</v>
       </c>
       <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
         <v>89</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,16 +1860,16 @@
         <v>2A</v>
       </c>
       <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
         <v>46</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1938,13 +1932,13 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" t="s">
         <v>85</v>
-      </c>
-      <c r="E55" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1967,10 +1961,10 @@
         <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -1986,10 +1980,10 @@
         <v>33</v>
       </c>
       <c r="C58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
@@ -2005,10 +1999,10 @@
         <v>34</v>
       </c>
       <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="s">
         <v>26</v>
-      </c>
-      <c r="D59" t="s">
-        <v>27</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
@@ -2024,7 +2018,7 @@
         <v>35</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
@@ -2053,10 +2047,10 @@
         <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2072,10 +2066,10 @@
         <v>38</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2091,10 +2085,10 @@
         <v>39</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2110,10 +2104,10 @@
         <v>3A</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2129,10 +2123,10 @@
         <v>3B</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2148,10 +2142,10 @@
         <v>3C</v>
       </c>
       <c r="C67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" t="s">
         <v>49</v>
-      </c>
-      <c r="D67" t="s">
-        <v>50</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
@@ -2219,7 +2213,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2235,16 +2229,16 @@
         <v>42</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2279,16 +2273,16 @@
         <v>45</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2321,7 +2315,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2343,7 +2337,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2389,10 +2383,10 @@
         <v>4C</v>
       </c>
       <c r="C83" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" t="s">
         <v>76</v>
-      </c>
-      <c r="D83" t="s">
-        <v>77</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2408,10 +2402,10 @@
         <v>4D</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2427,16 +2421,16 @@
         <v>4E</v>
       </c>
       <c r="C85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" t="s">
         <v>82</v>
-      </c>
-      <c r="D85" t="s">
-        <v>83</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2449,7 +2443,7 @@
         <v>4F</v>
       </c>
       <c r="D86" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,16 +2456,16 @@
         <v>50</v>
       </c>
       <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>74</v>
+      </c>
+      <c r="E87" t="s">
+        <v>110</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D87" t="s">
-        <v>75</v>
-      </c>
-      <c r="E87" t="s">
-        <v>111</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2484,16 +2478,16 @@
         <v>51</v>
       </c>
       <c r="C88" t="s">
+        <v>108</v>
+      </c>
+      <c r="D88" t="s">
         <v>109</v>
       </c>
-      <c r="D88" t="s">
-        <v>110</v>
-      </c>
       <c r="E88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,16 +2541,16 @@
         <v>56</v>
       </c>
       <c r="C93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2569,13 +2563,13 @@
         <v>57</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2588,13 +2582,13 @@
         <v>58</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,13 +2601,13 @@
         <v>59</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2626,13 +2620,13 @@
         <v>5A</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2645,13 +2639,13 @@
         <v>5B</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2664,13 +2658,13 @@
         <v>5C</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2683,13 +2677,13 @@
         <v>5D</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2702,13 +2696,13 @@
         <v>5E</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2721,13 +2715,13 @@
         <v>5F</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2740,13 +2734,13 @@
         <v>60</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2759,13 +2753,13 @@
         <v>61</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2778,13 +2772,13 @@
         <v>62</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2797,13 +2791,13 @@
         <v>63</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2816,13 +2810,13 @@
         <v>64</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2835,13 +2829,13 @@
         <v>65</v>
       </c>
       <c r="C108" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E108" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2923,6 +2917,18 @@
         <f t="shared" si="2"/>
         <v>6D</v>
       </c>
+      <c r="C116" t="s">
+        <v>151</v>
+      </c>
+      <c r="D116" t="s">
+        <v>18</v>
+      </c>
+      <c r="E116" t="s">
+        <v>19</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
@@ -3034,16 +3040,16 @@
         <v>78</v>
       </c>
       <c r="C127" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D127" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D127" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="E127" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3106,10 +3112,10 @@
         <v>7E</v>
       </c>
       <c r="C133" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D133" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3128,7 +3134,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
bugfixes in event handling, interface clock up to 25MHz
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="156">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -477,9 +477,6 @@
     <t>this also pulses the RAM read clk</t>
   </si>
   <si>
-    <t>write this register to initiate readout</t>
-  </si>
-  <si>
     <t>clear readout process (might be helpful if hanging)</t>
   </si>
   <si>
@@ -493,13 +490,28 @@
   </si>
   <si>
     <t>set read register</t>
+  </si>
+  <si>
+    <t>LSB enables phased trigger, LSB+1 enables ext trig out, LSB+2 enables ext trig in</t>
+  </si>
+  <si>
+    <t>x000003</t>
+  </si>
+  <si>
+    <t>trigger enables</t>
+  </si>
+  <si>
+    <t>keep 0x00 empty to avoid SPI-duplex R/W confusion</t>
+  </si>
+  <si>
+    <t>write this register to initiate single 4-byte SPI readout. NOTE: this function is also called by writing registers 35-38, 109</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,6 +543,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -636,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -684,6 +704,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,21 +1085,25 @@
       <c r="A7">
         <v>0</v>
       </c>
-      <c r="B7" s="14" t="str">
-        <f>DEC2HEX(A7,2)</f>
-        <v>00</v>
+      <c r="B7" s="31" t="str">
+        <f>"x" &amp; DEC2HEX(A7,2)</f>
+        <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="str">
-        <f t="shared" ref="B8:B71" si="0">DEC2HEX(A8,2)</f>
-        <v>01</v>
+      <c r="B8" s="31" t="str">
+        <f t="shared" ref="B8:B71" si="0">"x" &amp; DEC2HEX(A8,2)</f>
+        <v>x01</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1080,9 +1117,9 @@
         <f>1+A8</f>
         <v>2</v>
       </c>
-      <c r="B9" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>02</v>
+      <c r="B9" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x02</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -1096,9 +1133,9 @@
         <f t="shared" ref="A10:A73" si="1">1+A9</f>
         <v>3</v>
       </c>
-      <c r="B10" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>03</v>
+      <c r="B10" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x03</v>
       </c>
       <c r="C10" t="s">
         <v>91</v>
@@ -1112,9 +1149,9 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B11" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>04</v>
+      <c r="B11" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x04</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -1131,9 +1168,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B12" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>05</v>
+      <c r="B12" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x05</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -1150,9 +1187,9 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B13" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>06</v>
+      <c r="B13" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x06</v>
       </c>
       <c r="C13" t="s">
         <v>42</v>
@@ -1169,9 +1206,9 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B14" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>07</v>
+      <c r="B14" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x07</v>
       </c>
       <c r="C14" t="s">
         <v>83</v>
@@ -1180,7 +1217,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1188,9 +1225,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>08</v>
+      <c r="B15" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x08</v>
       </c>
       <c r="C15" t="s">
         <v>135</v>
@@ -1199,7 +1236,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1207,9 +1244,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>09</v>
+      <c r="B16" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x09</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>16</v>
@@ -1220,9 +1257,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B17" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>0A</v>
+      <c r="B17" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>x0A</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>95</v>
@@ -1242,9 +1279,9 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B18" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0B</v>
+      <c r="B18" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x0B</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>96</v>
@@ -1262,9 +1299,9 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B19" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0C</v>
+      <c r="B19" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x0C</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>97</v>
@@ -1282,9 +1319,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B20" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0D</v>
+      <c r="B20" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x0D</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>98</v>
@@ -1302,9 +1339,9 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B21" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0E</v>
+      <c r="B21" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x0E</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>99</v>
@@ -1322,9 +1359,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B22" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>0F</v>
+      <c r="B22" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x0F</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>100</v>
@@ -1342,9 +1379,9 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B23" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="B23" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x10</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>101</v>
@@ -1364,9 +1401,9 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B24" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
+      <c r="B24" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x11</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>113</v>
@@ -1386,9 +1423,9 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B25" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="B25" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x12</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>104</v>
@@ -1408,9 +1445,9 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B26" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>13</v>
+      <c r="B26" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x13</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>105</v>
@@ -1428,9 +1465,9 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B27" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>14</v>
+      <c r="B27" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x14</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>114</v>
@@ -1448,9 +1485,9 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B28" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>15</v>
+      <c r="B28" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x15</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>115</v>
@@ -1468,9 +1505,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B29" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="B29" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x16</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>122</v>
@@ -1488,9 +1525,9 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B30" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>17</v>
+      <c r="B30" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x17</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>121</v>
@@ -1508,9 +1545,9 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B31" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>18</v>
+      <c r="B31" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x18</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>123</v>
@@ -1528,9 +1565,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B32" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>19</v>
+      <c r="B32" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x19</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>116</v>
@@ -1548,9 +1585,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B33" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>1A</v>
+      <c r="B33" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x1A</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>117</v>
@@ -1568,9 +1605,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B34" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>1B</v>
+      <c r="B34" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x1B</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>118</v>
@@ -1588,9 +1625,9 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B35" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>1C</v>
+      <c r="B35" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x1C</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>119</v>
@@ -1608,9 +1645,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B36" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>1D</v>
+      <c r="B36" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x1D</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>120</v>
@@ -1628,9 +1665,9 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B37" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>1E</v>
+      <c r="B37" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x1E</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>124</v>
@@ -1648,9 +1685,9 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B38" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>1F</v>
+      <c r="B38" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x1F</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>125</v>
@@ -1668,9 +1705,9 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B39" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="B39" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x20</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>126</v>
@@ -1688,9 +1725,9 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B40" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="B40" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>x21</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>127</v>
@@ -1708,9 +1745,9 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B41" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>22</v>
+      <c r="B41" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>x22</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>128</v>
@@ -1728,9 +1765,9 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B42" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>23</v>
+      <c r="B42" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x23</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>137</v>
@@ -1747,9 +1784,9 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B43" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>24</v>
+      <c r="B43" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x24</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>138</v>
@@ -1766,9 +1803,9 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B44" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="B44" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x25</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>139</v>
@@ -1785,9 +1822,9 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B45" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>26</v>
+      <c r="B45" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x26</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>140</v>
@@ -1804,9 +1841,9 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B46" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="B46" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x27</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1814,9 +1851,9 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B47" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="B47" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x28</v>
       </c>
       <c r="C47" t="s">
         <v>87</v>
@@ -1833,9 +1870,9 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B48" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>29</v>
+      <c r="B48" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x29</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -1855,9 +1892,9 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B49" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>2A</v>
+      <c r="B49" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x2A</v>
       </c>
       <c r="C49" t="s">
         <v>45</v>
@@ -1877,9 +1914,9 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B50" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>2B</v>
+      <c r="B50" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x2B</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,9 +1924,9 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B51" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>2C</v>
+      <c r="B51" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x2C</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,9 +1934,9 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B52" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>2D</v>
+      <c r="B52" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x2D</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1907,9 +1944,9 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B53" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>2E</v>
+      <c r="B53" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x2E</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,9 +1954,9 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B54" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>2F</v>
+      <c r="B54" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x2F</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,9 +1964,9 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B55" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="B55" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x30</v>
       </c>
       <c r="C55" t="s">
         <v>51</v>
@@ -1946,9 +1983,9 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B56" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="B56" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x31</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,9 +1993,9 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B57" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="B57" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x32</v>
       </c>
       <c r="C57" t="s">
         <v>20</v>
@@ -1975,9 +2012,9 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B58" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>33</v>
+      <c r="B58" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x33</v>
       </c>
       <c r="C58" t="s">
         <v>24</v>
@@ -1994,9 +2031,9 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B59" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>34</v>
+      <c r="B59" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x34</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -2013,9 +2050,9 @@
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B60" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="B60" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x35</v>
       </c>
       <c r="C60" t="s">
         <v>21</v>
@@ -2032,9 +2069,9 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B61" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="B61" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x36</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,9 +2079,9 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B62" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>37</v>
+      <c r="B62" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x37</v>
       </c>
       <c r="C62" t="s">
         <v>27</v>
@@ -2061,9 +2098,9 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B63" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>38</v>
+      <c r="B63" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x38</v>
       </c>
       <c r="C63" t="s">
         <v>29</v>
@@ -2080,9 +2117,9 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B64" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>39</v>
+      <c r="B64" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x39</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>30</v>
@@ -2099,9 +2136,9 @@
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B65" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>3A</v>
+      <c r="B65" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x3A</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>31</v>
@@ -2118,9 +2155,9 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B66" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>3B</v>
+      <c r="B66" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x3B</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>32</v>
@@ -2137,9 +2174,9 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B67" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>3C</v>
+      <c r="B67" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x3C</v>
       </c>
       <c r="C67" t="s">
         <v>48</v>
@@ -2156,9 +2193,9 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B68" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>3D</v>
+      <c r="B68" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x3D</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2166,9 +2203,9 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B69" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>3E</v>
+      <c r="B69" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x3E</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2176,9 +2213,9 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B70" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>3F</v>
+      <c r="B70" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x3F</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2186,9 +2223,9 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B71" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="B71" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>x40</v>
       </c>
       <c r="C71" t="s">
         <v>10</v>
@@ -2205,9 +2242,9 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B72" s="14" t="str">
-        <f t="shared" ref="B72:B134" si="2">DEC2HEX(A72,2)</f>
-        <v>41</v>
+      <c r="B72" s="31" t="str">
+        <f t="shared" ref="B72:B134" si="2">"x" &amp; DEC2HEX(A72,2)</f>
+        <v>x41</v>
       </c>
       <c r="C72" t="s">
         <v>11</v>
@@ -2224,9 +2261,9 @@
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="B73" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>42</v>
+      <c r="B73" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x42</v>
       </c>
       <c r="C73" t="s">
         <v>38</v>
@@ -2246,9 +2283,9 @@
         <f t="shared" ref="A74:A134" si="3">1+A73</f>
         <v>67</v>
       </c>
-      <c r="B74" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>43</v>
+      <c r="B74" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x43</v>
       </c>
       <c r="F74" s="11"/>
     </row>
@@ -2257,9 +2294,9 @@
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="B75" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>44</v>
+      <c r="B75" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x44</v>
       </c>
       <c r="F75" s="11"/>
     </row>
@@ -2268,9 +2305,9 @@
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="B76" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>45</v>
+      <c r="B76" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x45</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>37</v>
@@ -2290,20 +2327,20 @@
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B77" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>46</v>
+      <c r="B77" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x46</v>
       </c>
       <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="B78" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>47</v>
+      <c r="B78" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x47</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>13</v>
@@ -2315,7 +2352,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2323,9 +2360,9 @@
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="B79" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>48</v>
+      <c r="B79" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x48</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>14</v>
@@ -2337,7 +2374,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2345,9 +2382,9 @@
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="B80" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>49</v>
+      <c r="B80" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x49</v>
       </c>
       <c r="E80" s="4"/>
     </row>
@@ -2356,9 +2393,9 @@
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="B81" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>4A</v>
+      <c r="B81" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x4A</v>
       </c>
       <c r="F81" s="11"/>
     </row>
@@ -2367,9 +2404,9 @@
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="B82" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>4B</v>
+      <c r="B82" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x4B</v>
       </c>
       <c r="F82" s="11"/>
     </row>
@@ -2378,9 +2415,9 @@
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="B83" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>4C</v>
+      <c r="B83" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x4C</v>
       </c>
       <c r="C83" t="s">
         <v>75</v>
@@ -2397,9 +2434,9 @@
         <f t="shared" si="3"/>
         <v>77</v>
       </c>
-      <c r="B84" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>4D</v>
+      <c r="B84" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x4D</v>
       </c>
       <c r="C84" t="s">
         <v>79</v>
@@ -2416,9 +2453,9 @@
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="B85" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>4E</v>
+      <c r="B85" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x4E</v>
       </c>
       <c r="C85" t="s">
         <v>81</v>
@@ -2438,9 +2475,9 @@
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="B86" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>4F</v>
+      <c r="B86" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x4F</v>
       </c>
       <c r="D86" t="s">
         <v>39</v>
@@ -2451,9 +2488,9 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="B87" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>50</v>
+      <c r="B87" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x50</v>
       </c>
       <c r="C87" t="s">
         <v>72</v>
@@ -2473,9 +2510,9 @@
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
-      <c r="B88" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>51</v>
+      <c r="B88" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x51</v>
       </c>
       <c r="C88" t="s">
         <v>108</v>
@@ -2495,9 +2532,18 @@
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="B89" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>52</v>
+      <c r="B89" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x52</v>
+      </c>
+      <c r="C89" t="s">
+        <v>153</v>
+      </c>
+      <c r="D89" t="s">
+        <v>151</v>
+      </c>
+      <c r="E89" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2505,9 +2551,9 @@
         <f t="shared" si="3"/>
         <v>83</v>
       </c>
-      <c r="B90" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>53</v>
+      <c r="B90" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x53</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2515,9 +2561,9 @@
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="B91" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>54</v>
+      <c r="B91" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x54</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,9 +2571,9 @@
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="B92" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>55</v>
+      <c r="B92" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x55</v>
       </c>
       <c r="E92" s="12"/>
     </row>
@@ -2536,9 +2582,9 @@
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="B93" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>56</v>
+      <c r="B93" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x56</v>
       </c>
       <c r="C93" t="s">
         <v>53</v>
@@ -2558,9 +2604,9 @@
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="B94" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>57</v>
+      <c r="B94" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x57</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>52</v>
@@ -2577,9 +2623,9 @@
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="B95" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>58</v>
+      <c r="B95" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x58</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>54</v>
@@ -2596,9 +2642,9 @@
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="B96" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>59</v>
+      <c r="B96" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x59</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>55</v>
@@ -2615,9 +2661,9 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B97" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>5A</v>
+      <c r="B97" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x5A</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>56</v>
@@ -2634,9 +2680,9 @@
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="B98" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>5B</v>
+      <c r="B98" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x5B</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>57</v>
@@ -2653,9 +2699,9 @@
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="B99" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>5C</v>
+      <c r="B99" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x5C</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>58</v>
@@ -2672,9 +2718,9 @@
         <f t="shared" si="3"/>
         <v>93</v>
       </c>
-      <c r="B100" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>5D</v>
+      <c r="B100" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x5D</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>59</v>
@@ -2691,9 +2737,9 @@
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="B101" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>5E</v>
+      <c r="B101" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x5E</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>60</v>
@@ -2710,9 +2756,9 @@
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="B102" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>5F</v>
+      <c r="B102" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x5F</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>61</v>
@@ -2729,9 +2775,9 @@
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="B103" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>60</v>
+      <c r="B103" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x60</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>62</v>
@@ -2748,9 +2794,9 @@
         <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="B104" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>61</v>
+      <c r="B104" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x61</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>63</v>
@@ -2767,9 +2813,9 @@
         <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="B105" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>62</v>
+      <c r="B105" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x62</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>64</v>
@@ -2786,9 +2832,9 @@
         <f t="shared" si="3"/>
         <v>99</v>
       </c>
-      <c r="B106" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>63</v>
+      <c r="B106" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x63</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>65</v>
@@ -2805,9 +2851,9 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="B107" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>64</v>
+      <c r="B107" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x64</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>66</v>
@@ -2824,9 +2870,9 @@
         <f t="shared" si="3"/>
         <v>101</v>
       </c>
-      <c r="B108" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>65</v>
+      <c r="B108" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x65</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>67</v>
@@ -2843,9 +2889,9 @@
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="B109" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>66</v>
+      <c r="B109" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x66</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,9 +2899,9 @@
         <f t="shared" si="3"/>
         <v>103</v>
       </c>
-      <c r="B110" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>67</v>
+      <c r="B110" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x67</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2863,9 +2909,9 @@
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="B111" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>68</v>
+      <c r="B111" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x68</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2873,9 +2919,9 @@
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="B112" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>69</v>
+      <c r="B112" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x69</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2883,9 +2929,9 @@
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
-      <c r="B113" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>6A</v>
+      <c r="B113" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x6A</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2893,9 +2939,9 @@
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
-      <c r="B114" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>6B</v>
+      <c r="B114" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x6B</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -2903,9 +2949,9 @@
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
-      <c r="B115" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>6C</v>
+      <c r="B115" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x6C</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2913,12 +2959,12 @@
         <f t="shared" si="3"/>
         <v>109</v>
       </c>
-      <c r="B116" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>6D</v>
+      <c r="B116" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D116" t="s">
         <v>18</v>
@@ -2935,9 +2981,9 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="B117" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>6E</v>
+      <c r="B117" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x6E</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -2945,9 +2991,9 @@
         <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="B118" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>6F</v>
+      <c r="B118" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x6F</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,9 +3001,9 @@
         <f t="shared" si="3"/>
         <v>112</v>
       </c>
-      <c r="B119" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>70</v>
+      <c r="B119" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x70</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -2965,9 +3011,9 @@
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="B120" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>71</v>
+      <c r="B120" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x71</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -2975,9 +3021,9 @@
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
-      <c r="B121" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>72</v>
+      <c r="B121" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x72</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,9 +3031,9 @@
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
-      <c r="B122" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>73</v>
+      <c r="B122" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x73</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -2995,9 +3041,9 @@
         <f t="shared" si="3"/>
         <v>116</v>
       </c>
-      <c r="B123" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>74</v>
+      <c r="B123" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x74</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3005,9 +3051,9 @@
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
-      <c r="B124" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>75</v>
+      <c r="B124" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x75</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3015,9 +3061,9 @@
         <f t="shared" si="3"/>
         <v>118</v>
       </c>
-      <c r="B125" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>76</v>
+      <c r="B125" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x76</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3025,9 +3071,9 @@
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
-      <c r="B126" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>77</v>
+      <c r="B126" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x77</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3035,9 +3081,9 @@
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B127" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>78</v>
+      <c r="B127" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x78</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>35</v>
@@ -3057,9 +3103,9 @@
         <f t="shared" si="3"/>
         <v>121</v>
       </c>
-      <c r="B128" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>79</v>
+      <c r="B128" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x79</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3067,9 +3113,9 @@
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="B129" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>7A</v>
+      <c r="B129" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x7A</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3077,9 +3123,9 @@
         <f t="shared" si="3"/>
         <v>123</v>
       </c>
-      <c r="B130" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>7B</v>
+      <c r="B130" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x7B</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3087,9 +3133,9 @@
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
-      <c r="B131" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>7C</v>
+      <c r="B131" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x7C</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,9 +3143,9 @@
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="B132" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>7D</v>
+      <c r="B132" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x7D</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3107,9 +3153,9 @@
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="B133" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>7E</v>
+      <c r="B133" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x7E</v>
       </c>
       <c r="C133" t="s">
         <v>94</v>
@@ -3126,9 +3172,9 @@
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="B134" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>7F</v>
+      <c r="B134" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>x7F</v>
       </c>
       <c r="C134" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Bug-free readout, working with external clock source
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>rdout-&gt;wfm readout chan</t>
+  </si>
+  <si>
+    <t>x000001</t>
   </si>
   <si>
     <t>address pulsed</t>
@@ -505,6 +508,9 @@
   </si>
   <si>
     <t>write this register to initiate single 4-byte SPI readout. NOTE: this function is also called by writing registers 35-38, 109</t>
+  </si>
+  <si>
+    <t>status reg-&gt; data manager [same mapping as reg 7, but only updated when pulsing register 77]</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,10 +1056,10 @@
       <c r="B4" s="26"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1067,7 +1073,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1076,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
@@ -1090,10 +1096,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1106,10 +1112,10 @@
         <v>x01</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1122,10 +1128,10 @@
         <v>x02</v>
       </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1138,10 +1144,10 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1154,13 +1160,13 @@
         <v>x04</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,13 +1179,13 @@
         <v>x05</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1192,13 +1198,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1211,13 +1217,13 @@
         <v>x07</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1230,16 +1236,16 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1248,8 +1254,11 @@
         <f t="shared" si="0"/>
         <v>x09</v>
       </c>
+      <c r="C16" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="D16" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,16 +1271,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1284,10 +1293,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>7</v>
@@ -1304,10 +1313,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>7</v>
@@ -1324,10 +1333,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>7</v>
@@ -1344,10 +1353,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>7</v>
@@ -1364,10 +1373,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>7</v>
@@ -1384,16 +1393,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1406,16 +1415,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1428,16 +1437,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1450,10 +1459,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>7</v>
@@ -1470,10 +1479,10 @@
         <v>x14</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>7</v>
@@ -1490,10 +1499,10 @@
         <v>x15</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>7</v>
@@ -1510,10 +1519,10 @@
         <v>x16</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>7</v>
@@ -1530,10 +1539,10 @@
         <v>x17</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>7</v>
@@ -1550,10 +1559,10 @@
         <v>x18</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>7</v>
@@ -1570,10 +1579,10 @@
         <v>x19</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>7</v>
@@ -1590,10 +1599,10 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>7</v>
@@ -1610,10 +1619,10 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>7</v>
@@ -1630,10 +1639,10 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>7</v>
@@ -1650,10 +1659,10 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>7</v>
@@ -1670,10 +1679,10 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>7</v>
@@ -1690,10 +1699,10 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>7</v>
@@ -1710,10 +1719,10 @@
         <v>x20</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>7</v>
@@ -1730,10 +1739,10 @@
         <v>x21</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>7</v>
@@ -1750,10 +1759,10 @@
         <v>x22</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>7</v>
@@ -1770,13 +1779,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,13 +1798,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,13 +1817,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1827,13 +1836,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,10 +1865,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
         <v>87</v>
-      </c>
-      <c r="D47" t="s">
-        <v>86</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1875,16 +1884,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
         <v>7</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,16 +1906,16 @@
         <v>x2A</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E49" t="s">
         <v>7</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1969,13 +1978,13 @@
         <v>x30</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,10 +2007,10 @@
         <v>x32</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -2017,10 +2026,10 @@
         <v>x33</v>
       </c>
       <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" t="s">
         <v>24</v>
-      </c>
-      <c r="D58" t="s">
-        <v>23</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
@@ -2036,10 +2045,10 @@
         <v>x34</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
@@ -2055,10 +2064,10 @@
         <v>x35</v>
       </c>
       <c r="C60" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E60" t="s">
         <v>7</v>
@@ -2084,10 +2093,10 @@
         <v>x37</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2103,10 +2112,10 @@
         <v>x38</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D63" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2122,10 +2131,10 @@
         <v>x39</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2141,10 +2150,10 @@
         <v>x3A</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2160,10 +2169,10 @@
         <v>x3B</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2179,10 +2188,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D67" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
@@ -2250,7 +2259,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2266,16 +2275,16 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2310,16 +2319,16 @@
         <v>x45</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2343,16 +2352,16 @@
         <v>x47</v>
       </c>
       <c r="C78" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>12</v>
       </c>
       <c r="E78" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2365,16 +2374,16 @@
         <v>x48</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F79" s="29" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2420,13 +2429,13 @@
         <v>x4C</v>
       </c>
       <c r="C83" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D83" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E83" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,10 +2448,10 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D84" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2458,16 +2467,16 @@
         <v>x4E</v>
       </c>
       <c r="C85" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D85" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2480,7 +2489,7 @@
         <v>x4F</v>
       </c>
       <c r="D86" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2493,16 +2502,16 @@
         <v>x50</v>
       </c>
       <c r="C87" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D87" t="s">
+        <v>75</v>
+      </c>
+      <c r="E87" t="s">
+        <v>111</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="E87" t="s">
-        <v>110</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2515,16 +2524,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D88" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E88" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2537,13 +2546,13 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
+        <v>154</v>
+      </c>
+      <c r="D89" t="s">
+        <v>152</v>
+      </c>
+      <c r="E89" t="s">
         <v>153</v>
-      </c>
-      <c r="D89" t="s">
-        <v>151</v>
-      </c>
-      <c r="E89" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2587,16 +2596,16 @@
         <v>x56</v>
       </c>
       <c r="C93" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D93" t="s">
+        <v>70</v>
+      </c>
+      <c r="E93" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E93" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="F93" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2609,13 +2618,13 @@
         <v>x57</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D94" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E94" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E94" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,13 +2637,13 @@
         <v>x58</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D95" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E95" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2647,13 +2656,13 @@
         <v>x59</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D96" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E96" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E96" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,13 +2675,13 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D97" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E97" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E97" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2685,13 +2694,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D98" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E98" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E98" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,13 +2713,13 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D99" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E99" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E99" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2723,13 +2732,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D100" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E100" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E100" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2742,13 +2751,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D101" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E101" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E101" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2761,13 +2770,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D102" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E102" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2780,13 +2789,13 @@
         <v>x60</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D103" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E103" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E103" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2799,13 +2808,13 @@
         <v>x61</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D104" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E104" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E104" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2818,13 +2827,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D105" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E105" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E105" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2837,13 +2846,13 @@
         <v>x63</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D106" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E106" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E106" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2856,13 +2865,13 @@
         <v>x64</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D107" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E107" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E107" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,13 +2884,13 @@
         <v>x65</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D108" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E108" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2964,16 +2973,16 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D116" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E116" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3086,16 +3095,16 @@
         <v>x78</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3158,10 +3167,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D133" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3180,7 +3189,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add external trig functionality
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="162">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -495,9 +494,6 @@
     <t>set read register</t>
   </si>
   <si>
-    <t>LSB enables phased trigger, LSB+1 enables ext trig out, LSB+2 enables ext trig in</t>
-  </si>
-  <si>
     <t>x000003</t>
   </si>
   <si>
@@ -511,6 +507,21 @@
   </si>
   <si>
     <t>status reg-&gt; data manager [same mapping as reg 7, but only updated when pulsing register 77]</t>
+  </si>
+  <si>
+    <t>external trigger output config</t>
+  </si>
+  <si>
+    <t>x000033</t>
+  </si>
+  <si>
+    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; enable external trig input to external trig output ; bits 8 to 15-&gt;width as specified by 25 MHz clock cycles</t>
+  </si>
+  <si>
+    <t>default width of 120 ns</t>
+  </si>
+  <si>
+    <t>LSB enables phased trigger, LSB+1 enables ext trig in</t>
   </si>
 </sst>
 </file>
@@ -686,7 +697,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -702,8 +712,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -724,6 +732,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,45 +1026,45 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="14" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="80.85546875" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="33">
         <v>42917</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>79</v>
@@ -1091,15 +1102,15 @@
       <c r="A7">
         <v>0</v>
       </c>
-      <c r="B7" s="31" t="str">
+      <c r="B7" s="28" t="str">
         <f>"x" &amp; DEC2HEX(A7,2)</f>
         <v>x00</v>
       </c>
       <c r="C7" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>155</v>
+      <c r="D7" s="27" t="s">
+        <v>154</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1107,7 +1118,7 @@
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="31" t="str">
+      <c r="B8" s="28" t="str">
         <f t="shared" ref="B8:B71" si="0">"x" &amp; DEC2HEX(A8,2)</f>
         <v>x01</v>
       </c>
@@ -1123,7 +1134,7 @@
         <f>1+A8</f>
         <v>2</v>
       </c>
-      <c r="B9" s="31" t="str">
+      <c r="B9" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x02</v>
       </c>
@@ -1139,7 +1150,7 @@
         <f t="shared" ref="A10:A73" si="1">1+A9</f>
         <v>3</v>
       </c>
-      <c r="B10" s="31" t="str">
+      <c r="B10" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x03</v>
       </c>
@@ -1155,7 +1166,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B11" s="31" t="str">
+      <c r="B11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x04</v>
       </c>
@@ -1174,7 +1185,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B12" s="31" t="str">
+      <c r="B12" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x05</v>
       </c>
@@ -1193,7 +1204,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B13" s="31" t="str">
+      <c r="B13" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x06</v>
       </c>
@@ -1212,7 +1223,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B14" s="31" t="str">
+      <c r="B14" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x07</v>
       </c>
@@ -1231,7 +1242,7 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B15" s="31" t="str">
+      <c r="B15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x08</v>
       </c>
@@ -1250,541 +1261,541 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B16" s="31" t="str">
+      <c r="B16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B17" s="32" t="str">
+      <c r="B17" s="29" t="str">
         <f t="shared" si="0"/>
         <v>x0A</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="E17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B18" s="33" t="str">
+      <c r="B18" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x0B</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="21"/>
+      <c r="E18" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B19" s="33" t="str">
+      <c r="B19" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x0C</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="21"/>
+      <c r="E19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B20" s="33" t="str">
+      <c r="B20" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x0D</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="21"/>
+      <c r="E20" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="A21" s="18">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B21" s="33" t="str">
+      <c r="B21" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x0E</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="21"/>
+      <c r="E21" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="18">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B22" s="33" t="str">
+      <c r="B22" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x0F</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="21"/>
+      <c r="E22" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="18">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B23" s="33" t="str">
+      <c r="B23" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x10</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="21" t="s">
+      <c r="E23" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="18">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B24" s="33" t="str">
+      <c r="B24" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x11</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="21" t="s">
+      <c r="E24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+      <c r="A25" s="18">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B25" s="33" t="str">
+      <c r="B25" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x12</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="21" t="s">
+      <c r="E25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="18">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B26" s="33" t="str">
+      <c r="B26" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x13</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="21"/>
+      <c r="E26" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="18">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B27" s="33" t="str">
+      <c r="B27" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x14</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="21"/>
+      <c r="E27" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="18">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B28" s="33" t="str">
+      <c r="B28" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x15</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="21"/>
+      <c r="E28" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
+      <c r="A29" s="18">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B29" s="33" t="str">
+      <c r="B29" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x16</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="21"/>
+      <c r="E29" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="18">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B30" s="33" t="str">
+      <c r="B30" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x17</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="21"/>
+      <c r="E30" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="20"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+      <c r="A31" s="18">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B31" s="33" t="str">
+      <c r="B31" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x18</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="21"/>
+      <c r="E31" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="18">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B32" s="33" t="str">
+      <c r="B32" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x19</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="21"/>
+      <c r="E32" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
+      <c r="A33" s="18">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B33" s="33" t="str">
+      <c r="B33" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x1A</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="18">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B34" s="33" t="str">
+      <c r="B34" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x1B</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="20"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
+      <c r="A35" s="18">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B35" s="33" t="str">
+      <c r="B35" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x1C</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="20"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
+      <c r="A36" s="18">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B36" s="33" t="str">
+      <c r="B36" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x1D</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="20"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
+      <c r="A37" s="18">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B37" s="33" t="str">
+      <c r="B37" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x1E</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="21"/>
+      <c r="E37" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+      <c r="A38" s="18">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B38" s="33" t="str">
+      <c r="B38" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x1F</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="21"/>
+      <c r="E38" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="20"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
+      <c r="A39" s="18">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B39" s="33" t="str">
+      <c r="B39" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x20</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="21"/>
+      <c r="E39" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
+      <c r="A40" s="18">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B40" s="33" t="str">
+      <c r="B40" s="30" t="str">
         <f t="shared" si="0"/>
         <v>x21</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="21"/>
+      <c r="E40" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="20"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
+      <c r="A41" s="21">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B41" s="34" t="str">
+      <c r="B41" s="31" t="str">
         <f t="shared" si="0"/>
         <v>x22</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="24"/>
+      <c r="E41" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B42" s="31" t="str">
+      <c r="B42" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x23</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="F42" s="28" t="s">
+      <c r="F42" s="25" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1793,17 +1804,17 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B43" s="31" t="str">
+      <c r="B43" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x24</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="27" t="s">
+      <c r="D43" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="F43" s="28" t="s">
+      <c r="F43" s="25" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1812,17 +1823,17 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B44" s="31" t="str">
+      <c r="B44" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x25</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="D44" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="25" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1831,17 +1842,17 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B45" s="31" t="str">
+      <c r="B45" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x26</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D45" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="F45" s="28" t="s">
+      <c r="F45" s="25" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1850,7 +1861,7 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B46" s="31" t="str">
+      <c r="B46" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x27</v>
       </c>
@@ -1860,7 +1871,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B47" s="31" t="str">
+      <c r="B47" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x28</v>
       </c>
@@ -1879,7 +1890,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B48" s="31" t="str">
+      <c r="B48" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x29</v>
       </c>
@@ -1901,7 +1912,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B49" s="31" t="str">
+      <c r="B49" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x2A</v>
       </c>
@@ -1923,7 +1934,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B50" s="31" t="str">
+      <c r="B50" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x2B</v>
       </c>
@@ -1933,7 +1944,7 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B51" s="31" t="str">
+      <c r="B51" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x2C</v>
       </c>
@@ -1943,7 +1954,7 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B52" s="31" t="str">
+      <c r="B52" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x2D</v>
       </c>
@@ -1953,7 +1964,7 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B53" s="31" t="str">
+      <c r="B53" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x2E</v>
       </c>
@@ -1963,7 +1974,7 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B54" s="31" t="str">
+      <c r="B54" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x2F</v>
       </c>
@@ -1973,7 +1984,7 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B55" s="31" t="str">
+      <c r="B55" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x30</v>
       </c>
@@ -1992,7 +2003,7 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B56" s="31" t="str">
+      <c r="B56" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x31</v>
       </c>
@@ -2002,7 +2013,7 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B57" s="31" t="str">
+      <c r="B57" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x32</v>
       </c>
@@ -2021,7 +2032,7 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B58" s="31" t="str">
+      <c r="B58" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x33</v>
       </c>
@@ -2040,7 +2051,7 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B59" s="31" t="str">
+      <c r="B59" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x34</v>
       </c>
@@ -2059,7 +2070,7 @@
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B60" s="31" t="str">
+      <c r="B60" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x35</v>
       </c>
@@ -2078,7 +2089,7 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B61" s="31" t="str">
+      <c r="B61" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x36</v>
       </c>
@@ -2088,7 +2099,7 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B62" s="31" t="str">
+      <c r="B62" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x37</v>
       </c>
@@ -2107,7 +2118,7 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B63" s="31" t="str">
+      <c r="B63" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x38</v>
       </c>
@@ -2126,7 +2137,7 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B64" s="31" t="str">
+      <c r="B64" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x39</v>
       </c>
@@ -2145,7 +2156,7 @@
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B65" s="31" t="str">
+      <c r="B65" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3A</v>
       </c>
@@ -2164,7 +2175,7 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B66" s="31" t="str">
+      <c r="B66" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3B</v>
       </c>
@@ -2183,7 +2194,7 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B67" s="31" t="str">
+      <c r="B67" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3C</v>
       </c>
@@ -2202,7 +2213,7 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B68" s="31" t="str">
+      <c r="B68" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3D</v>
       </c>
@@ -2212,7 +2223,7 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B69" s="31" t="str">
+      <c r="B69" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3E</v>
       </c>
@@ -2222,7 +2233,7 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B70" s="31" t="str">
+      <c r="B70" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3F</v>
       </c>
@@ -2232,7 +2243,7 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B71" s="31" t="str">
+      <c r="B71" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x40</v>
       </c>
@@ -2251,7 +2262,7 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B72" s="31" t="str">
+      <c r="B72" s="28" t="str">
         <f t="shared" ref="B72:B134" si="2">"x" &amp; DEC2HEX(A72,2)</f>
         <v>x41</v>
       </c>
@@ -2270,7 +2281,7 @@
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="B73" s="31" t="str">
+      <c r="B73" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x42</v>
       </c>
@@ -2292,7 +2303,7 @@
         <f t="shared" ref="A74:A134" si="3">1+A73</f>
         <v>67</v>
       </c>
-      <c r="B74" s="31" t="str">
+      <c r="B74" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x43</v>
       </c>
@@ -2303,7 +2314,7 @@
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="B75" s="31" t="str">
+      <c r="B75" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x44</v>
       </c>
@@ -2314,7 +2325,7 @@
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="B76" s="31" t="str">
+      <c r="B76" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x45</v>
       </c>
@@ -2336,7 +2347,7 @@
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B77" s="31" t="str">
+      <c r="B77" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x46</v>
       </c>
@@ -2347,7 +2358,7 @@
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="B78" s="31" t="str">
+      <c r="B78" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x47</v>
       </c>
@@ -2361,7 +2372,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2369,7 +2380,7 @@
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="B79" s="31" t="str">
+      <c r="B79" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x48</v>
       </c>
@@ -2382,7 +2393,7 @@
       <c r="E79" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F79" s="29" t="s">
+      <c r="F79" s="26" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2391,7 +2402,7 @@
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="B80" s="31" t="str">
+      <c r="B80" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x49</v>
       </c>
@@ -2402,7 +2413,7 @@
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="B81" s="31" t="str">
+      <c r="B81" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x4A</v>
       </c>
@@ -2413,7 +2424,7 @@
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="B82" s="31" t="str">
+      <c r="B82" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x4B</v>
       </c>
@@ -2424,7 +2435,7 @@
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="B83" s="31" t="str">
+      <c r="B83" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x4C</v>
       </c>
@@ -2443,7 +2454,7 @@
         <f t="shared" si="3"/>
         <v>77</v>
       </c>
-      <c r="B84" s="31" t="str">
+      <c r="B84" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x4D</v>
       </c>
@@ -2462,7 +2473,7 @@
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="B85" s="31" t="str">
+      <c r="B85" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x4E</v>
       </c>
@@ -2484,7 +2495,7 @@
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="B86" s="31" t="str">
+      <c r="B86" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x4F</v>
       </c>
@@ -2497,7 +2508,7 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="B87" s="31" t="str">
+      <c r="B87" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x50</v>
       </c>
@@ -2519,7 +2530,7 @@
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
-      <c r="B88" s="31" t="str">
+      <c r="B88" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x51</v>
       </c>
@@ -2541,28 +2552,40 @@
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="B89" s="31" t="str">
+      <c r="B89" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D89" t="s">
+        <v>161</v>
+      </c>
+      <c r="E89" t="s">
         <v>152</v>
       </c>
-      <c r="E89" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="3"/>
         <v>83</v>
       </c>
-      <c r="B90" s="31" t="str">
+      <c r="B90" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x53</v>
+      </c>
+      <c r="C90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E90" t="s">
+        <v>158</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2570,7 +2593,7 @@
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="B91" s="31" t="str">
+      <c r="B91" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x54</v>
       </c>
@@ -2580,7 +2603,7 @@
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="B92" s="31" t="str">
+      <c r="B92" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
@@ -2591,7 +2614,7 @@
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="B93" s="31" t="str">
+      <c r="B93" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x56</v>
       </c>
@@ -2613,7 +2636,7 @@
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="B94" s="31" t="str">
+      <c r="B94" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x57</v>
       </c>
@@ -2632,7 +2655,7 @@
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="B95" s="31" t="str">
+      <c r="B95" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x58</v>
       </c>
@@ -2651,7 +2674,7 @@
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="B96" s="31" t="str">
+      <c r="B96" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x59</v>
       </c>
@@ -2670,7 +2693,7 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B97" s="31" t="str">
+      <c r="B97" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x5A</v>
       </c>
@@ -2689,7 +2712,7 @@
         <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="B98" s="31" t="str">
+      <c r="B98" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x5B</v>
       </c>
@@ -2708,7 +2731,7 @@
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="B99" s="31" t="str">
+      <c r="B99" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x5C</v>
       </c>
@@ -2727,7 +2750,7 @@
         <f t="shared" si="3"/>
         <v>93</v>
       </c>
-      <c r="B100" s="31" t="str">
+      <c r="B100" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x5D</v>
       </c>
@@ -2746,7 +2769,7 @@
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="B101" s="31" t="str">
+      <c r="B101" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x5E</v>
       </c>
@@ -2765,7 +2788,7 @@
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="B102" s="31" t="str">
+      <c r="B102" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x5F</v>
       </c>
@@ -2784,7 +2807,7 @@
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="B103" s="31" t="str">
+      <c r="B103" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x60</v>
       </c>
@@ -2803,7 +2826,7 @@
         <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="B104" s="31" t="str">
+      <c r="B104" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x61</v>
       </c>
@@ -2822,7 +2845,7 @@
         <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="B105" s="31" t="str">
+      <c r="B105" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x62</v>
       </c>
@@ -2841,7 +2864,7 @@
         <f t="shared" si="3"/>
         <v>99</v>
       </c>
-      <c r="B106" s="31" t="str">
+      <c r="B106" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x63</v>
       </c>
@@ -2860,7 +2883,7 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="B107" s="31" t="str">
+      <c r="B107" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x64</v>
       </c>
@@ -2879,7 +2902,7 @@
         <f t="shared" si="3"/>
         <v>101</v>
       </c>
-      <c r="B108" s="31" t="str">
+      <c r="B108" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x65</v>
       </c>
@@ -2898,7 +2921,7 @@
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="B109" s="31" t="str">
+      <c r="B109" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x66</v>
       </c>
@@ -2908,7 +2931,7 @@
         <f t="shared" si="3"/>
         <v>103</v>
       </c>
-      <c r="B110" s="31" t="str">
+      <c r="B110" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x67</v>
       </c>
@@ -2918,7 +2941,7 @@
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="B111" s="31" t="str">
+      <c r="B111" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x68</v>
       </c>
@@ -2928,7 +2951,7 @@
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="B112" s="31" t="str">
+      <c r="B112" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x69</v>
       </c>
@@ -2938,7 +2961,7 @@
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
-      <c r="B113" s="31" t="str">
+      <c r="B113" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x6A</v>
       </c>
@@ -2948,7 +2971,7 @@
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
-      <c r="B114" s="31" t="str">
+      <c r="B114" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x6B</v>
       </c>
@@ -2958,7 +2981,7 @@
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
-      <c r="B115" s="31" t="str">
+      <c r="B115" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x6C</v>
       </c>
@@ -2968,7 +2991,7 @@
         <f t="shared" si="3"/>
         <v>109</v>
       </c>
-      <c r="B116" s="31" t="str">
+      <c r="B116" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x6D</v>
       </c>
@@ -2990,7 +3013,7 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="B117" s="31" t="str">
+      <c r="B117" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x6E</v>
       </c>
@@ -3000,7 +3023,7 @@
         <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="B118" s="31" t="str">
+      <c r="B118" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x6F</v>
       </c>
@@ -3010,7 +3033,7 @@
         <f t="shared" si="3"/>
         <v>112</v>
       </c>
-      <c r="B119" s="31" t="str">
+      <c r="B119" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x70</v>
       </c>
@@ -3020,7 +3043,7 @@
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="B120" s="31" t="str">
+      <c r="B120" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x71</v>
       </c>
@@ -3030,7 +3053,7 @@
         <f t="shared" si="3"/>
         <v>114</v>
       </c>
-      <c r="B121" s="31" t="str">
+      <c r="B121" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x72</v>
       </c>
@@ -3040,7 +3063,7 @@
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
-      <c r="B122" s="31" t="str">
+      <c r="B122" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x73</v>
       </c>
@@ -3050,7 +3073,7 @@
         <f t="shared" si="3"/>
         <v>116</v>
       </c>
-      <c r="B123" s="31" t="str">
+      <c r="B123" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x74</v>
       </c>
@@ -3060,7 +3083,7 @@
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
-      <c r="B124" s="31" t="str">
+      <c r="B124" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x75</v>
       </c>
@@ -3070,7 +3093,7 @@
         <f t="shared" si="3"/>
         <v>118</v>
       </c>
-      <c r="B125" s="31" t="str">
+      <c r="B125" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x76</v>
       </c>
@@ -3080,7 +3103,7 @@
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
-      <c r="B126" s="31" t="str">
+      <c r="B126" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x77</v>
       </c>
@@ -3090,7 +3113,7 @@
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B127" s="31" t="str">
+      <c r="B127" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x78</v>
       </c>
@@ -3112,7 +3135,7 @@
         <f t="shared" si="3"/>
         <v>121</v>
       </c>
-      <c r="B128" s="31" t="str">
+      <c r="B128" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x79</v>
       </c>
@@ -3122,7 +3145,7 @@
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="B129" s="31" t="str">
+      <c r="B129" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x7A</v>
       </c>
@@ -3132,7 +3155,7 @@
         <f t="shared" si="3"/>
         <v>123</v>
       </c>
-      <c r="B130" s="31" t="str">
+      <c r="B130" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x7B</v>
       </c>
@@ -3142,7 +3165,7 @@
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
-      <c r="B131" s="31" t="str">
+      <c r="B131" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x7C</v>
       </c>
@@ -3152,7 +3175,7 @@
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="B132" s="31" t="str">
+      <c r="B132" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x7D</v>
       </c>
@@ -3162,7 +3185,7 @@
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="B133" s="31" t="str">
+      <c r="B133" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x7E</v>
       </c>
@@ -3181,7 +3204,7 @@
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="B134" s="31" t="str">
+      <c r="B134" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x7F</v>
       </c>

</xml_diff>

<commit_message>
add master/slave register syncing feature
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="165">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -512,9 +513,6 @@
     <t>external trigger output config</t>
   </si>
   <si>
-    <t>x000033</t>
-  </si>
-  <si>
     <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; enable external trig input to external trig output ; bits 8 to 15-&gt;width as specified by 25 MHz clock cycles</t>
   </si>
   <si>
@@ -522,6 +520,18 @@
   </si>
   <si>
     <t>LSB enables phased trigger, LSB+1 enables ext trig in</t>
+  </si>
+  <si>
+    <t>x000303</t>
+  </si>
+  <si>
+    <t>sync command</t>
+  </si>
+  <si>
+    <t>write  a 1 to lsb to enable hold, writing a 0 to lsb after hold releases a sync</t>
+  </si>
+  <si>
+    <t>write only / MASTER board only</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1865,6 +1875,18 @@
         <f t="shared" si="0"/>
         <v>x27</v>
       </c>
+      <c r="C46" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -2560,7 +2582,7 @@
         <v>153</v>
       </c>
       <c r="D89" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E89" t="s">
         <v>152</v>
@@ -2579,13 +2601,13 @@
         <v>157</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90" t="s">
+        <v>161</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="E90" t="s">
-        <v>158</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cleaning up, allow beams to be turned off/on
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="166">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -495,9 +495,6 @@
     <t>set read register</t>
   </si>
   <si>
-    <t>x000003</t>
-  </si>
-  <si>
     <t>trigger enables</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t>default width of 120 ns</t>
   </si>
   <si>
-    <t>LSB enables phased trigger, LSB+1 enables ext trig in</t>
-  </si>
-  <si>
     <t>x000303</t>
   </si>
   <si>
@@ -532,6 +526,15 @@
   </si>
   <si>
     <t>write only / MASTER board only</t>
+  </si>
+  <si>
+    <t>LSB enables phased trigger; LSB+1 enables ext trig in; bits 2 thru 4 enable beams 8, 4a,4b, respectively</t>
+  </si>
+  <si>
+    <t>x00001E</t>
+  </si>
+  <si>
+    <t>default: phased trigger disabled at startup (LSB)</t>
   </si>
 </sst>
 </file>
@@ -1027,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1123,7 @@
         <v>150</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1276,7 +1279,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1876,16 +1879,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="D46" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D46" s="24" t="s">
-        <v>164</v>
-      </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2394,7 +2397,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2569,7 +2572,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -2579,13 +2582,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>153</v>
-      </c>
-      <c r="D89" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="E89" t="s">
-        <v>152</v>
+        <v>164</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2598,16 +2604,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>156</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" t="s">
+        <v>159</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E90" t="s">
-        <v>161</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding master/slave sync, working ext trig
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -180,21 +180,6 @@
     <t>lower 4 bits set PD (I+Q channel, ADCs 0-&gt;3)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">lower bit only -- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">EVENTUALLY SWITCH DEFAULT TO EXTERNAL </t>
-    </r>
-  </si>
-  <si>
     <t>channel mask</t>
   </si>
   <si>
@@ -348,9 +333,6 @@
     <t>metadata-&gt;deadtime counter</t>
   </si>
   <si>
-    <t>deadtime counter refreshed every second</t>
-  </si>
-  <si>
     <t>note: metadata assigned to these registers once event buffer set in register 78</t>
   </si>
   <si>
@@ -535,13 +517,19 @@
   </si>
   <si>
     <t>default: phased trigger disabled at startup (LSB)</t>
+  </si>
+  <si>
+    <t>Default external reference clock</t>
+  </si>
+  <si>
+    <t>deadtime counter (num 25 MHz clk cycles) refreshed every second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,13 +548,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -708,7 +689,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -732,7 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1030,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1061,7 @@
       <c r="B4" s="34"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
@@ -1097,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1120,10 +1101,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1168,7 +1149,7 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1187,10 +1168,10 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1206,7 +1187,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>44</v>
@@ -1225,7 +1206,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>45</v>
@@ -1241,13 +1222,13 @@
         <v>x07</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1260,13 +1241,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1279,7 +1260,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1295,16 +1276,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,10 +1298,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>7</v>
@@ -1337,10 +1318,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>7</v>
@@ -1357,10 +1338,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>7</v>
@@ -1377,10 +1358,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>7</v>
@@ -1397,10 +1378,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>7</v>
@@ -1417,16 +1398,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1439,16 +1420,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1461,16 +1442,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>105</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,10 +1464,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>7</v>
@@ -1503,7 +1484,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1523,7 +1504,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1543,7 +1524,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1563,7 +1544,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1583,7 +1564,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1603,7 +1584,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1623,7 +1604,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1643,7 +1624,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1663,7 +1644,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1683,7 +1664,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1703,7 +1684,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1723,7 +1704,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1743,7 +1724,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1763,7 +1744,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1783,7 +1764,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1803,13 +1784,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1822,13 +1803,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1841,13 +1822,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="25" t="s">
         <v>140</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,13 +1841,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1879,16 +1860,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="D46" s="24" t="s">
-        <v>162</v>
-      </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1901,10 +1882,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1920,16 +1901,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
         <v>89</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2014,13 +1995,13 @@
         <v>x30</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" t="s">
         <v>85</v>
-      </c>
-      <c r="E55" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2132,7 +2113,7 @@
         <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2295,7 +2276,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2314,13 +2295,13 @@
         <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2358,13 +2339,13 @@
         <v>38</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2397,7 +2378,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2419,7 +2400,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2465,10 +2446,10 @@
         <v>x4C</v>
       </c>
       <c r="C83" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" t="s">
         <v>76</v>
-      </c>
-      <c r="D83" t="s">
-        <v>77</v>
       </c>
       <c r="E83" t="s">
         <v>12</v>
@@ -2484,10 +2465,10 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D84" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2503,16 +2484,16 @@
         <v>x4E</v>
       </c>
       <c r="C85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" t="s">
         <v>82</v>
-      </c>
-      <c r="D85" t="s">
-        <v>83</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2538,16 +2519,16 @@
         <v>x50</v>
       </c>
       <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>74</v>
+      </c>
+      <c r="E87" t="s">
+        <v>109</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D87" t="s">
-        <v>75</v>
-      </c>
-      <c r="E87" t="s">
-        <v>111</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2560,16 +2541,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D88" t="s">
+        <v>108</v>
+      </c>
+      <c r="E88" t="s">
         <v>110</v>
       </c>
-      <c r="E88" t="s">
-        <v>112</v>
-      </c>
       <c r="F88" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2582,16 +2563,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E89" t="s">
+        <v>162</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="E89" t="s">
-        <v>164</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2604,16 +2585,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>154</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E90" t="s">
+        <v>157</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E90" t="s">
-        <v>159</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2647,16 +2628,16 @@
         <v>x56</v>
       </c>
       <c r="C93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2669,13 +2650,13 @@
         <v>x57</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2688,13 +2669,13 @@
         <v>x58</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2707,13 +2688,13 @@
         <v>x59</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,13 +2707,13 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2745,13 +2726,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2764,13 +2745,13 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2783,13 +2764,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2802,13 +2783,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2821,13 +2802,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2840,13 +2821,13 @@
         <v>x60</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2859,13 +2840,13 @@
         <v>x61</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2878,13 +2859,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2897,13 +2878,13 @@
         <v>x63</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2916,13 +2897,13 @@
         <v>x64</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,13 +2916,13 @@
         <v>x65</v>
       </c>
       <c r="C108" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E108" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3024,7 +3005,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3033,7 +3014,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3152,10 +3133,10 @@
         <v>37</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3218,10 +3199,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D133" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3240,7 +3221,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
various updates, uptick version to 1.2
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="167">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -138,9 +138,6 @@
     <t>clock select</t>
   </si>
   <si>
-    <t>master 100 MHz clock select: local oscillator (==1) or external LVDS input (==0)</t>
-  </si>
-  <si>
     <t>rdout-&gt;ram address</t>
   </si>
   <si>
@@ -526,6 +523,9 @@
   </si>
   <si>
     <t>functionality to reset buffer to zero only works if not currently saving an event.</t>
+  </si>
+  <si>
+    <t>LSB: master 100 MHz clock select: local oscillator (==1) or external LVDS input (==0)</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D79" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
       <c r="B4" s="34"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
@@ -1081,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1104,10 +1104,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1152,7 +1152,7 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1168,13 +1168,13 @@
         <v>x04</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,13 +1187,13 @@
         <v>x05</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1206,13 +1206,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1225,13 +1225,13 @@
         <v>x07</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1244,13 +1244,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1263,7 +1263,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1279,16 +1279,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,10 +1301,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>7</v>
@@ -1321,10 +1321,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>7</v>
@@ -1341,10 +1341,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>7</v>
@@ -1361,10 +1361,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>7</v>
@@ -1381,10 +1381,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>7</v>
@@ -1401,16 +1401,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1423,16 +1423,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,16 +1445,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,10 +1467,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>7</v>
@@ -1487,7 +1487,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1507,7 +1507,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1527,7 +1527,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1547,7 +1547,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1567,7 +1567,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1587,7 +1587,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1607,7 +1607,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1627,7 +1627,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1647,7 +1647,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1667,7 +1667,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1687,7 +1687,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1707,7 +1707,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1727,7 +1727,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1747,7 +1747,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1767,7 +1767,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1787,13 +1787,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,13 +1806,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,13 +1825,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1844,13 +1844,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F45" s="25" t="s">
         <v>137</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1863,16 +1863,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,10 +1885,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1904,16 +1904,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
         <v>87</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1926,16 +1926,16 @@
         <v>x2A</v>
       </c>
       <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
         <v>46</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,13 +1998,13 @@
         <v>x30</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D55" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" t="s">
         <v>83</v>
-      </c>
-      <c r="E55" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
         <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2208,10 +2208,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" t="s">
         <v>49</v>
-      </c>
-      <c r="D67" t="s">
-        <v>50</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
@@ -2279,7 +2279,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2295,16 +2295,16 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2339,16 +2339,16 @@
         <v>x45</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2449,10 +2449,10 @@
         <v>x4C</v>
       </c>
       <c r="C83" t="s">
+        <v>74</v>
+      </c>
+      <c r="D83" t="s">
         <v>75</v>
-      </c>
-      <c r="D83" t="s">
-        <v>76</v>
       </c>
       <c r="E83" t="s">
         <v>12</v>
@@ -2468,16 +2468,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84" t="s">
         <v>164</v>
-      </c>
-      <c r="D84" t="s">
-        <v>165</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2490,16 +2490,16 @@
         <v>x4E</v>
       </c>
       <c r="C85" t="s">
+        <v>79</v>
+      </c>
+      <c r="D85" t="s">
         <v>80</v>
-      </c>
-      <c r="D85" t="s">
-        <v>81</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2512,7 +2512,7 @@
         <v>x4F</v>
       </c>
       <c r="D86" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,16 +2525,16 @@
         <v>x50</v>
       </c>
       <c r="C87" t="s">
+        <v>71</v>
+      </c>
+      <c r="D87" t="s">
+        <v>73</v>
+      </c>
+      <c r="E87" t="s">
+        <v>107</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="D87" t="s">
-        <v>74</v>
-      </c>
-      <c r="E87" t="s">
-        <v>108</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,16 +2547,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
+        <v>105</v>
+      </c>
+      <c r="D88" t="s">
         <v>106</v>
       </c>
-      <c r="D88" t="s">
-        <v>107</v>
-      </c>
       <c r="E88" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2569,16 +2569,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E89" t="s">
         <v>159</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2591,16 +2591,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" t="s">
+        <v>154</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="E90" t="s">
-        <v>155</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2634,16 +2634,16 @@
         <v>x56</v>
       </c>
       <c r="C93" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2656,13 +2656,13 @@
         <v>x57</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,13 +2675,13 @@
         <v>x58</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2694,13 +2694,13 @@
         <v>x59</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2713,13 +2713,13 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2732,13 +2732,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2751,13 +2751,13 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2770,13 +2770,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,13 +2789,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2808,13 +2808,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,13 +2827,13 @@
         <v>x60</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2846,13 +2846,13 @@
         <v>x61</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2865,13 +2865,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2884,13 +2884,13 @@
         <v>x63</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2903,13 +2903,13 @@
         <v>x64</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2922,13 +2922,13 @@
         <v>x65</v>
       </c>
       <c r="C108" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E108" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3011,7 +3011,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3020,7 +3020,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3136,13 +3136,13 @@
         <v>36</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3205,10 +3205,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D133" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3227,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
found bug in beamformer
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -129,9 +129,6 @@
     <t>adc-&gt;serdes delay ADC3</t>
   </si>
   <si>
-    <t>lower 4 bits set delay</t>
-  </si>
-  <si>
     <t>power-up default value</t>
   </si>
   <si>
@@ -526,6 +523,9 @@
   </si>
   <si>
     <t>LSB: master 100 MHz clock select: local oscillator (==1) or external LVDS input (==0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bits 0-3 [8-11] set delay on CH0 [CH1], bit 4 [12] enables delay on CH0 [CH1], bit 5 [13] adds entire extra clk cycle of delay on CH0 [CH1] </t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
       <c r="B4" s="34"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
@@ -1081,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1090,7 +1090,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
@@ -1104,10 +1104,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1152,7 +1152,7 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1168,13 +1168,13 @@
         <v>x04</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,13 +1187,13 @@
         <v>x05</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1206,13 +1206,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1225,13 +1225,13 @@
         <v>x07</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1244,13 +1244,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1263,7 +1263,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1279,16 +1279,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,10 +1301,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>7</v>
@@ -1321,10 +1321,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>7</v>
@@ -1341,10 +1341,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>7</v>
@@ -1361,10 +1361,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>7</v>
@@ -1381,10 +1381,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>7</v>
@@ -1401,16 +1401,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1423,16 +1423,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,16 +1445,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,10 +1467,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>7</v>
@@ -1487,7 +1487,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1507,7 +1507,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1527,7 +1527,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1547,7 +1547,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1567,7 +1567,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1587,7 +1587,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1607,7 +1607,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1627,7 +1627,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1647,7 +1647,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1667,7 +1667,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1687,7 +1687,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1707,7 +1707,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1727,7 +1727,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1747,7 +1747,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1767,7 +1767,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1787,13 +1787,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,13 +1806,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,13 +1825,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1844,13 +1844,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1863,16 +1863,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,10 +1885,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1904,16 +1904,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
         <v>86</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1926,16 +1926,16 @@
         <v>x2A</v>
       </c>
       <c r="C49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" t="s">
         <v>45</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,13 +1998,13 @@
         <v>x30</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
         <v>82</v>
-      </c>
-      <c r="E55" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2116,13 +2116,13 @@
         <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2134,14 +2134,14 @@
       <c r="C63" t="s">
         <v>30</v>
       </c>
-      <c r="D63" t="s">
-        <v>34</v>
+      <c r="D63" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2153,14 +2153,14 @@
       <c r="C64" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>34</v>
+      <c r="D64" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2172,14 +2172,14 @@
       <c r="C65" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>34</v>
+      <c r="D65" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -2191,8 +2191,8 @@
       <c r="C66" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>34</v>
+      <c r="D66" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2208,10 +2208,10 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" t="s">
         <v>48</v>
-      </c>
-      <c r="D67" t="s">
-        <v>49</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
@@ -2279,7 +2279,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2295,16 +2295,16 @@
         <v>x42</v>
       </c>
       <c r="C73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2339,16 +2339,16 @@
         <v>x45</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2449,10 +2449,10 @@
         <v>x4C</v>
       </c>
       <c r="C83" t="s">
+        <v>73</v>
+      </c>
+      <c r="D83" t="s">
         <v>74</v>
-      </c>
-      <c r="D83" t="s">
-        <v>75</v>
       </c>
       <c r="E83" t="s">
         <v>12</v>
@@ -2468,16 +2468,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>162</v>
+      </c>
+      <c r="D84" t="s">
         <v>163</v>
-      </c>
-      <c r="D84" t="s">
-        <v>164</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2490,16 +2490,16 @@
         <v>x4E</v>
       </c>
       <c r="C85" t="s">
+        <v>78</v>
+      </c>
+      <c r="D85" t="s">
         <v>79</v>
-      </c>
-      <c r="D85" t="s">
-        <v>80</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2512,7 +2512,7 @@
         <v>x4F</v>
       </c>
       <c r="D86" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,16 +2525,16 @@
         <v>x50</v>
       </c>
       <c r="C87" t="s">
+        <v>70</v>
+      </c>
+      <c r="D87" t="s">
+        <v>72</v>
+      </c>
+      <c r="E87" t="s">
+        <v>106</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D87" t="s">
-        <v>73</v>
-      </c>
-      <c r="E87" t="s">
-        <v>107</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,16 +2547,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
+        <v>104</v>
+      </c>
+      <c r="D88" t="s">
         <v>105</v>
       </c>
-      <c r="D88" t="s">
-        <v>106</v>
-      </c>
       <c r="E88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2569,16 +2569,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E89" t="s">
         <v>158</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2591,16 +2591,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>150</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" t="s">
+        <v>153</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="E90" t="s">
-        <v>154</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2634,16 +2634,16 @@
         <v>x56</v>
       </c>
       <c r="C93" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2656,13 +2656,13 @@
         <v>x57</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,13 +2675,13 @@
         <v>x58</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2694,13 +2694,13 @@
         <v>x59</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2713,13 +2713,13 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2732,13 +2732,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2751,13 +2751,13 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2770,13 +2770,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,13 +2789,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2808,13 +2808,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,13 +2827,13 @@
         <v>x60</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2846,13 +2846,13 @@
         <v>x61</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2865,13 +2865,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2884,13 +2884,13 @@
         <v>x63</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2903,13 +2903,13 @@
         <v>x64</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2922,13 +2922,13 @@
         <v>x65</v>
       </c>
       <c r="C108" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3011,7 +3011,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3020,7 +3020,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3133,16 +3133,16 @@
         <v>x78</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3205,10 +3205,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D133" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3227,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add enable for phased trigger applied to data-saving
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="170">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -526,6 +526,15 @@
   </si>
   <si>
     <t xml:space="preserve">bits 0-3 [8-11] set delay on CH0 [CH1], bit 4 [12] enables delay on CH0 [CH1], bit 5 [13] adds entire extra clk cycle of delay on CH0 [CH1] </t>
+  </si>
+  <si>
+    <t>enable phased trigger to trigger data manager</t>
+  </si>
+  <si>
+    <t>LSB-&gt;enable</t>
+  </si>
+  <si>
+    <t>allows the scalers to be run without triggering the data manager, disabling allows easy initilization of the data manager paramters</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,7 +2612,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -2611,6 +2620,18 @@
       <c r="B91" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x54</v>
+      </c>
+      <c r="C91" t="s">
+        <v>167</v>
+      </c>
+      <c r="D91" t="s">
+        <v>168</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bugfixes, tick version to 1.4, trig timestamp now on 93.75MHz clk
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="175">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -342,9 +342,6 @@
     <t>trigger holdoff</t>
   </si>
   <si>
-    <t>set trigger holdoff (this is applied to each beam, sets earliest re-trigger time in each beam)</t>
-  </si>
-  <si>
     <t>xFFFFFF</t>
   </si>
   <si>
@@ -535,6 +532,24 @@
   </si>
   <si>
     <t>allows the scalers to be run without triggering the data manager, disabling allows easy initilization of the data manager paramters</t>
+  </si>
+  <si>
+    <t>SEE SCALER SHEET (**TO DO**)</t>
+  </si>
+  <si>
+    <t>default on slave board is 0x00000C (ADCs 2 and 3 off by default)</t>
+  </si>
+  <si>
+    <t>trigger holdoff mode</t>
+  </si>
+  <si>
+    <t>LSB=1 : trigger hold off value is global, LSB=0: trigger hold off value is per beam</t>
+  </si>
+  <si>
+    <t>choose between holdoff blocking all beam triggers (DEFAULT MODE), or just the specific triggered beam</t>
+  </si>
+  <si>
+    <t>set trigger holdoff (sets earliest re-trigger time in each beam [if 85 LSB=0] or global re-trigger time [if 85 LSB=1])</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1105,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1113,10 +1128,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1166,6 +1181,9 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
+      <c r="F10" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1183,7 +1201,7 @@
         <v>75</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1240,7 +1258,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1253,13 +1271,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1272,7 +1290,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1419,7 +1437,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1432,7 +1450,7 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>90</v>
@@ -1441,7 +1459,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1496,7 +1514,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1516,7 +1534,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1536,7 +1554,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1556,7 +1574,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1576,7 +1594,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1596,7 +1614,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1616,7 +1634,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1636,7 +1654,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1656,7 +1674,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1676,7 +1694,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1696,7 +1714,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1716,7 +1734,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1736,7 +1754,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1756,7 +1774,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1776,7 +1794,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1796,13 +1814,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1815,13 +1833,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,13 +1852,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1853,13 +1871,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="25" t="s">
         <v>135</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,16 +1890,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,7 +2162,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2163,7 +2181,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2182,7 +2200,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2201,7 +2219,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2224,6 +2242,9 @@
       </c>
       <c r="E67" t="s">
         <v>7</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2288,7 +2309,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2351,13 +2372,13 @@
         <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2390,7 +2411,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2412,7 +2433,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2477,16 +2498,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>161</v>
+      </c>
+      <c r="D84" t="s">
         <v>162</v>
-      </c>
-      <c r="D84" t="s">
-        <v>163</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,7 +2529,7 @@
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2540,13 +2561,13 @@
         <v>72</v>
       </c>
       <c r="E87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -2558,14 +2579,14 @@
       <c r="C88" t="s">
         <v>104</v>
       </c>
-      <c r="D88" t="s">
-        <v>105</v>
+      <c r="D88" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="E88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2578,16 +2599,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E89" t="s">
         <v>157</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2600,16 +2621,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>149</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" t="s">
+        <v>152</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="E90" t="s">
-        <v>153</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2622,19 +2643,19 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" t="s">
         <v>167</v>
-      </c>
-      <c r="D91" t="s">
-        <v>168</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -2643,7 +2664,18 @@
         <f t="shared" si="2"/>
         <v>x55</v>
       </c>
-      <c r="E92" s="12"/>
+      <c r="C92" t="s">
+        <v>171</v>
+      </c>
+      <c r="D92" t="s">
+        <v>172</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
@@ -2664,7 +2696,7 @@
         <v>66</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3032,7 +3064,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3041,7 +3073,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3157,13 +3189,13 @@
         <v>35</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix beam power output assignment
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="179">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -504,9 +504,6 @@
     <t>default: phased trigger disabled at startup (LSB)</t>
   </si>
   <si>
-    <t>Default external reference clock</t>
-  </si>
-  <si>
     <t>deadtime counter (num 25 MHz clk cycles) refreshed every second</t>
   </si>
   <si>
@@ -550,6 +547,21 @@
   </si>
   <si>
     <t>set trigger holdoff (sets earliest re-trigger time in each beam [if 85 LSB=0] or global re-trigger time [if 85 LSB=1])</t>
+  </si>
+  <si>
+    <t>Default external reference clock (don’t touch this register unless an emergency)</t>
+  </si>
+  <si>
+    <t>default min attenuation</t>
+  </si>
+  <si>
+    <t>block/allow channels in beam-forming</t>
+  </si>
+  <si>
+    <t>x000004</t>
+  </si>
+  <si>
+    <t>Default updated 9/1/2017 and tested: puts triggered pulse at beginning of readout window</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1194,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,7 +1449,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2033,6 +2045,9 @@
       <c r="E55" t="s">
         <v>82</v>
       </c>
+      <c r="F55" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -2062,6 +2077,9 @@
       <c r="E57" t="s">
         <v>7</v>
       </c>
+      <c r="F57" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -2081,6 +2099,9 @@
       <c r="E58" t="s">
         <v>7</v>
       </c>
+      <c r="F58" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -2100,6 +2121,9 @@
       <c r="E59" t="s">
         <v>7</v>
       </c>
+      <c r="F59" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -2162,7 +2186,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2181,7 +2205,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2200,7 +2224,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2219,7 +2243,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2244,7 +2268,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,7 +2493,7 @@
       </c>
       <c r="F82" s="11"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -2485,7 +2509,10 @@
         <v>74</v>
       </c>
       <c r="E83" t="s">
-        <v>12</v>
+        <v>177</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2498,16 +2525,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>160</v>
+      </c>
+      <c r="D84" t="s">
         <v>161</v>
-      </c>
-      <c r="D84" t="s">
-        <v>162</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2580,7 +2607,7 @@
         <v>104</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E88" t="s">
         <v>106</v>
@@ -2643,16 +2670,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91" t="s">
         <v>166</v>
-      </c>
-      <c r="D91" t="s">
-        <v>167</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2665,16 +2692,16 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" t="s">
         <v>171</v>
-      </c>
-      <c r="D92" t="s">
-        <v>172</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,13 +3216,13 @@
         <v>35</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add waveform-railing in beamforming to keep power within range
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="179">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -504,9 +504,6 @@
     <t>default: phased trigger disabled at startup (LSB)</t>
   </si>
   <si>
-    <t>Default external reference clock</t>
-  </si>
-  <si>
     <t>deadtime counter (num 25 MHz clk cycles) refreshed every second</t>
   </si>
   <si>
@@ -550,6 +547,21 @@
   </si>
   <si>
     <t>set trigger holdoff (sets earliest re-trigger time in each beam [if 85 LSB=0] or global re-trigger time [if 85 LSB=1])</t>
+  </si>
+  <si>
+    <t>Default external reference clock (don’t touch this register unless an emergency)</t>
+  </si>
+  <si>
+    <t>default min attenuation</t>
+  </si>
+  <si>
+    <t>block/allow channels in beam-forming</t>
+  </si>
+  <si>
+    <t>x000004</t>
+  </si>
+  <si>
+    <t>Default updated 9/1/2017 and tested: puts triggered pulse at beginning of readout window</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1194,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,7 +1449,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2033,6 +2045,9 @@
       <c r="E55" t="s">
         <v>82</v>
       </c>
+      <c r="F55" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -2062,6 +2077,9 @@
       <c r="E57" t="s">
         <v>7</v>
       </c>
+      <c r="F57" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -2081,6 +2099,9 @@
       <c r="E58" t="s">
         <v>7</v>
       </c>
+      <c r="F58" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -2100,6 +2121,9 @@
       <c r="E59" t="s">
         <v>7</v>
       </c>
+      <c r="F59" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -2162,7 +2186,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2181,7 +2205,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2200,7 +2224,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2219,7 +2243,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2244,7 +2268,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,7 +2493,7 @@
       </c>
       <c r="F82" s="11"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -2485,7 +2509,10 @@
         <v>74</v>
       </c>
       <c r="E83" t="s">
-        <v>12</v>
+        <v>177</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2498,16 +2525,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>160</v>
+      </c>
+      <c r="D84" t="s">
         <v>161</v>
-      </c>
-      <c r="D84" t="s">
-        <v>162</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2580,7 +2607,7 @@
         <v>104</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E88" t="s">
         <v>106</v>
@@ -2643,16 +2670,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91" t="s">
         <v>166</v>
-      </c>
-      <c r="D91" t="s">
-        <v>167</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2665,16 +2692,16 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" t="s">
         <v>171</v>
-      </c>
-      <c r="D92" t="s">
-        <v>172</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,13 +3216,13 @@
         <v>35</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add fpga core temp, update doc
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="183">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -150,15 +149,9 @@
     <t>chip_id(mid)</t>
   </si>
   <si>
-    <t>chip_id(high)</t>
-  </si>
-  <si>
     <t>mid 24 bits</t>
   </si>
   <si>
-    <t>high 16 bits</t>
-  </si>
-  <si>
     <t>cal pulser board</t>
   </si>
   <si>
@@ -562,6 +555,24 @@
   </si>
   <si>
     <t>Default updated 9/1/2017 and tested: puts triggered pulse at beginning of readout window</t>
+  </si>
+  <si>
+    <t>chip_id(high) + fpga temperature</t>
+  </si>
+  <si>
+    <t>read_only - board DNA (FPGA silicon-specific ID) + temperature</t>
+  </si>
+  <si>
+    <t>bit 23 downto 16: fpga temp (8 bits) ; bit 15 downto 0 : high 16 bits of chipID</t>
+  </si>
+  <si>
+    <t>update fpga temp sensor</t>
+  </si>
+  <si>
+    <t>better to keep disabled when not using to limit power consumption of ADC</t>
+  </si>
+  <si>
+    <t>write LSB to update, set LSB+1 to '1' to enable</t>
   </si>
 </sst>
 </file>
@@ -706,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -765,6 +776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1050,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,41 +1078,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="34">
         <v>42917</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
@@ -1117,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1140,10 +1152,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1188,13 +1200,13 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1210,10 +1222,10 @@
         <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1229,10 +1241,10 @@
         <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1245,13 +1257,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1264,13 +1276,13 @@
         <v>x07</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1283,13 +1295,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1302,7 +1314,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1318,16 +1330,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1340,10 +1352,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>7</v>
@@ -1360,10 +1372,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>7</v>
@@ -1380,10 +1392,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>7</v>
@@ -1400,10 +1412,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>7</v>
@@ -1420,10 +1432,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>7</v>
@@ -1440,16 +1452,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1462,16 +1474,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1484,16 +1496,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1506,10 +1518,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>7</v>
@@ -1526,7 +1538,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1546,7 +1558,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1566,7 +1578,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1586,7 +1598,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1606,7 +1618,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1626,7 +1638,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1646,7 +1658,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1666,7 +1678,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1686,7 +1698,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1706,7 +1718,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1726,7 +1738,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1746,7 +1758,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1766,7 +1778,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1786,7 +1798,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1806,7 +1818,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1826,13 +1838,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,13 +1857,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,13 +1876,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" s="25" t="s">
         <v>133</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1883,13 +1895,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,16 +1914,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="D46" s="24" t="s">
-        <v>155</v>
-      </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,10 +1936,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1943,16 +1955,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="D48" t="s">
-        <v>86</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,16 +1977,16 @@
         <v>x2A</v>
       </c>
       <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="D49" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2037,16 +2049,16 @@
         <v>x30</v>
       </c>
       <c r="C55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2078,7 +2090,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2100,7 +2112,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2122,7 +2134,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2167,7 +2179,7 @@
         <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2186,7 +2198,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2205,7 +2217,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2224,7 +2236,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2243,7 +2255,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2259,16 +2271,16 @@
         <v>x3C</v>
       </c>
       <c r="C67" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D67" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2333,7 +2345,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2352,13 +2364,13 @@
         <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2396,13 +2408,13 @@
         <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2435,7 +2447,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2457,7 +2469,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2503,16 +2515,16 @@
         <v>x4C</v>
       </c>
       <c r="C83" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D83" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E83" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,16 +2537,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D84" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,16 +2559,16 @@
         <v>x4E</v>
       </c>
       <c r="C85" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D85" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2582,16 +2594,16 @@
         <v>x50</v>
       </c>
       <c r="C87" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" t="s">
         <v>70</v>
       </c>
-      <c r="D87" t="s">
-        <v>72</v>
-      </c>
       <c r="E87" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2604,16 +2616,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
+        <v>102</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E88" t="s">
         <v>104</v>
       </c>
-      <c r="D88" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E88" t="s">
-        <v>106</v>
-      </c>
       <c r="F88" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2626,16 +2638,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E89" t="s">
+        <v>155</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="E89" t="s">
-        <v>157</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2648,16 +2660,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>147</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E90" t="s">
+        <v>150</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E90" t="s">
-        <v>152</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2670,16 +2682,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2692,16 +2704,16 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D92" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2714,16 +2726,16 @@
         <v>x56</v>
       </c>
       <c r="C93" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D93" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2736,13 +2748,13 @@
         <v>x57</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,13 +2767,13 @@
         <v>x58</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2774,13 +2786,13 @@
         <v>x59</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2793,13 +2805,13 @@
         <v>x5A</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2812,13 +2824,13 @@
         <v>x5B</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2831,13 +2843,13 @@
         <v>x5C</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2850,13 +2862,13 @@
         <v>x5D</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2869,13 +2881,13 @@
         <v>x5E</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2888,13 +2900,13 @@
         <v>x5F</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2907,13 +2919,13 @@
         <v>x60</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,13 +2938,13 @@
         <v>x61</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2945,13 +2957,13 @@
         <v>x62</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2964,13 +2976,13 @@
         <v>x63</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,13 +2995,13 @@
         <v>x64</v>
       </c>
       <c r="C107" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E107" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E107" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3002,13 +3014,13 @@
         <v>x65</v>
       </c>
       <c r="C108" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D108" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D108" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="E108" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3080,6 +3092,18 @@
         <f t="shared" si="2"/>
         <v>x6C</v>
       </c>
+      <c r="C115" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
@@ -3091,7 +3115,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3100,7 +3124,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3216,13 +3240,13 @@
         <v>35</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,10 +3309,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D133" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3307,7 +3331,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated trigger, with beam power 'verification'
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="182">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -398,9 +398,6 @@
     <t>start thresholds off at max (20 bits)</t>
   </si>
   <si>
-    <t>lower 12 bits -&gt; max trig hold off is 4095 * 1/(93.75 MHz) = 43.7 microsecs</t>
-  </si>
-  <si>
     <t>bits 23-22 : event buffer ; bit 21 : cal pulse switch ; bits 19-17 : pretrig window ; bits 16-15: trig type [0=nothing,1=software,2=phased trig,3=external] ; bits 14-0: last beam trigger</t>
   </si>
   <si>
@@ -530,18 +527,6 @@
     <t>default on slave board is 0x00000C (ADCs 2 and 3 off by default)</t>
   </si>
   <si>
-    <t>trigger holdoff mode</t>
-  </si>
-  <si>
-    <t>LSB=1 : trigger hold off value is global, LSB=0: trigger hold off value is per beam</t>
-  </si>
-  <si>
-    <t>choose between holdoff blocking all beam triggers (DEFAULT MODE), or just the specific triggered beam</t>
-  </si>
-  <si>
-    <t>set trigger holdoff (sets earliest re-trigger time in each beam [if 85 LSB=0] or global re-trigger time [if 85 LSB=1])</t>
-  </si>
-  <si>
     <t>Default external reference clock (don’t touch this register unless an emergency)</t>
   </si>
   <si>
@@ -573,6 +558,18 @@
   </si>
   <si>
     <t>write LSB to update, set LSB+1 to '1' to enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set trigger holdoff </t>
+  </si>
+  <si>
+    <t>lower 16 bits -&gt; max trig hold off is 2^16 * 1/(93.75 MHz) = 709 microsecs</t>
+  </si>
+  <si>
+    <t>trigger verification mode</t>
+  </si>
+  <si>
+    <t>LSB=1 : double checks that max beam is the trigger beam (+16 clock cycles of latency), LSB=0: trigger without verification</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1152,10 +1149,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1206,7 +1203,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1257,13 +1254,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1282,7 +1279,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1295,13 +1292,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1314,7 +1311,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1461,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1483,7 +1480,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1838,13 +1835,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,13 +1854,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,13 +1873,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1895,13 +1892,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="25" t="s">
         <v>132</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,16 +1911,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2058,7 +2055,7 @@
         <v>80</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2112,7 +2109,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2134,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,7 +2195,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2217,7 +2214,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2236,7 +2233,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2255,7 +2252,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2280,7 +2277,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2345,7 +2342,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2408,13 +2405,13 @@
         <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2447,7 +2444,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,7 +2466,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2521,10 +2518,10 @@
         <v>72</v>
       </c>
       <c r="E83" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2537,16 +2534,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>157</v>
+      </c>
+      <c r="D84" t="s">
         <v>158</v>
-      </c>
-      <c r="D84" t="s">
-        <v>159</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2606,7 +2603,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -2619,13 +2616,13 @@
         <v>102</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E88" t="s">
         <v>104</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2638,16 +2635,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E89" t="s">
         <v>154</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2660,16 +2657,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>146</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" t="s">
+        <v>149</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="E90" t="s">
-        <v>150</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2682,16 +2679,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>162</v>
+      </c>
+      <c r="D91" t="s">
         <v>163</v>
-      </c>
-      <c r="D91" t="s">
-        <v>164</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2704,17 +2701,14 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
-        <v>168</v>
-      </c>
-      <c r="D92" t="s">
-        <v>169</v>
+        <v>180</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F92" s="5" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
@@ -3093,16 +3087,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E115" s="32" t="s">
         <v>7</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3115,7 +3109,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3124,7 +3118,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3240,13 +3234,13 @@
         <v>35</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add remote firmware update functionality
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="200">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -570,6 +570,60 @@
   </si>
   <si>
     <t>LSB=1 : double checks that max beam is the trigger beam (+16 clock cycles of latency), LSB=0: trigger without verification</t>
+  </si>
+  <si>
+    <t>bit 0 write enable, bit 1 toggle fifo write clock</t>
+  </si>
+  <si>
+    <t>bits 15 to 0</t>
+  </si>
+  <si>
+    <t>LSB=0 : REMOTE update blocks in reset, commands ignored. Set to 1 to run.</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(0)-&gt; enable/reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMOTE UPDATE(1) -&gt; write enable to EPCQ fifo </t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(2) -&gt; write data to EPCQ fifo (lower 16 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(3) -&gt; write data to EPCQ fifo (upper 16 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(5) -&gt; write data to EPCQ cmd addr (lower 16 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(6) -&gt; write data to EPCQ cmd addr (upper 16 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(4) -&gt; EPCQ command / write mode / clear</t>
+  </si>
+  <si>
+    <t>cmd - bits 2 to 0 ; mode - bit 8 ; clear - bit 16</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(7) -&gt; remote update param, toggle_write, reconfig</t>
+  </si>
+  <si>
+    <t>bits 2 to 0 - param ; bit 8 - toggle_write ; bit 16 - reconfig</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(8) -&gt; remote update data (lower 16 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(9) -&gt; remote update data (upper 16 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE RD ONLY-&gt; status</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE RD ONLY-&gt; data low</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE RD ONLY-&gt; data high</t>
   </si>
 </sst>
 </file>
@@ -714,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -773,6 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -1059,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,38 +1130,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+      <c r="A4" s="35">
         <v>42917</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>74</v>
@@ -3036,6 +3091,9 @@
         <f t="shared" si="2"/>
         <v>x67</v>
       </c>
+      <c r="C110" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
@@ -3046,6 +3104,9 @@
         <f t="shared" si="2"/>
         <v>x68</v>
       </c>
+      <c r="C111" s="33" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
@@ -3056,6 +3117,9 @@
         <f t="shared" si="2"/>
         <v>x69</v>
       </c>
+      <c r="C112" s="33" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
@@ -3130,6 +3194,12 @@
         <f t="shared" si="2"/>
         <v>x6E</v>
       </c>
+      <c r="C117" t="s">
+        <v>185</v>
+      </c>
+      <c r="D117" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
@@ -3140,6 +3210,12 @@
         <f t="shared" si="2"/>
         <v>x6F</v>
       </c>
+      <c r="C118" t="s">
+        <v>186</v>
+      </c>
+      <c r="D118" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
@@ -3150,6 +3226,12 @@
         <f t="shared" si="2"/>
         <v>x70</v>
       </c>
+      <c r="C119" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="D119" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
@@ -3160,6 +3242,12 @@
         <f t="shared" si="2"/>
         <v>x71</v>
       </c>
+      <c r="C120" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D120" s="33" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
@@ -3170,6 +3258,12 @@
         <f t="shared" si="2"/>
         <v>x72</v>
       </c>
+      <c r="C121" t="s">
+        <v>191</v>
+      </c>
+      <c r="D121" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
@@ -3180,6 +3274,12 @@
         <f t="shared" si="2"/>
         <v>x73</v>
       </c>
+      <c r="C122" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D122" s="33" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
@@ -3190,6 +3290,12 @@
         <f t="shared" si="2"/>
         <v>x74</v>
       </c>
+      <c r="C123" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D123" s="33" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
@@ -3200,6 +3306,12 @@
         <f t="shared" si="2"/>
         <v>x75</v>
       </c>
+      <c r="C124" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D124" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
@@ -3210,6 +3322,12 @@
         <f t="shared" si="2"/>
         <v>x76</v>
       </c>
+      <c r="C125" t="s">
+        <v>195</v>
+      </c>
+      <c r="D125" s="33" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
@@ -3219,6 +3337,12 @@
       <c r="B126" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x77</v>
+      </c>
+      <c r="C126" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D126" s="33" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Increase wfm buffer to 2.3 microsecs, tick to ver1.8
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="206">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -624,6 +624,24 @@
   </si>
   <si>
     <t>REMOTE UPDATE RD ONLY-&gt; data high</t>
+  </si>
+  <si>
+    <t>bit 0 : enable, bit 1 : clk</t>
+  </si>
+  <si>
+    <t>(0):RU busy ; (1): EPCQ busy ; (2) EPCQ done ; (3) FIFO rd  empty ; (4) FIFO wr full</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE RD ONLY-&gt; epcq data low</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE RD ONLY-&gt; epcq data high</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(10) -&gt; EPCQ read RAM addr (lower 12 bits)</t>
+  </si>
+  <si>
+    <t>REMOTE UPDATE(11) -&gt; EPCQ read RAM clk/enable</t>
   </si>
 </sst>
 </file>
@@ -768,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -827,6 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1114,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,38 +1149,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
+      <c r="A4" s="36">
         <v>42917</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>74</v>
@@ -3094,6 +3113,9 @@
       <c r="C110" t="s">
         <v>197</v>
       </c>
+      <c r="D110" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
@@ -3130,6 +3152,9 @@
         <f t="shared" si="2"/>
         <v>x6A</v>
       </c>
+      <c r="C113" s="34" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
@@ -3140,6 +3165,9 @@
         <f t="shared" si="2"/>
         <v>x6B</v>
       </c>
+      <c r="C114" s="34" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
@@ -3354,17 +3382,8 @@
         <f t="shared" si="2"/>
         <v>x78</v>
       </c>
-      <c r="C127" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E127" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>167</v>
+      <c r="C127" s="34" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3376,8 +3395,14 @@
         <f t="shared" si="2"/>
         <v>x79</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>205</v>
+      </c>
+      <c r="D128" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -3387,7 +3412,7 @@
         <v>x7A</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -3397,7 +3422,7 @@
         <v>x7B</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -3406,8 +3431,20 @@
         <f t="shared" si="2"/>
         <v>x7C</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C131" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -3417,7 +3454,7 @@
         <v>x7D</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -3436,7 +3473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>127</v>

</xml_diff>

<commit_message>
add latched timestamp on ext trigger (i.e. PPS), update doc
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="214">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -269,12 +269,6 @@
     <t>0x0000FF</t>
   </si>
   <si>
-    <t>write a 1 to LSB to save scaler values</t>
-  </si>
-  <si>
-    <t>update scalers</t>
-  </si>
-  <si>
     <t>pick scaler to read</t>
   </si>
   <si>
@@ -338,9 +332,6 @@
     <t>xFFFFFF</t>
   </si>
   <si>
-    <t>x00000F</t>
-  </si>
-  <si>
     <t>chip ID is 64 bits: lower 24 bits</t>
   </si>
   <si>
@@ -452,9 +443,6 @@
     <t>set read register</t>
   </si>
   <si>
-    <t>trigger enables</t>
-  </si>
-  <si>
     <t>keep 0x00 empty to avoid SPI-duplex R/W confusion</t>
   </si>
   <si>
@@ -467,9 +455,6 @@
     <t>external trigger output config</t>
   </si>
   <si>
-    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; enable external trig input to external trig output ; bits 8 to 15-&gt;width as specified by 25 MHz clock cycles</t>
-  </si>
-  <si>
     <t>default width of 120 ns</t>
   </si>
   <si>
@@ -485,12 +470,6 @@
     <t>write only / MASTER board only</t>
   </si>
   <si>
-    <t>LSB enables phased trigger; LSB+1 enables ext trig in; bits 2 thru 4 enable beams 8, 4a,4b, respectively</t>
-  </si>
-  <si>
-    <t>x00001E</t>
-  </si>
-  <si>
     <t>default: phased trigger disabled at startup (LSB)</t>
   </si>
   <si>
@@ -642,6 +621,51 @@
   </si>
   <si>
     <t>REMOTE UPDATE(11) -&gt; EPCQ read RAM clk/enable</t>
+  </si>
+  <si>
+    <t>phased trigger enables</t>
+  </si>
+  <si>
+    <t>LSB enables phased trigger;  bits 8 thru 10 enable beams 8, 4a,4b, respectively</t>
+  </si>
+  <si>
+    <t>external trigger input config</t>
+  </si>
+  <si>
+    <t>x000700</t>
+  </si>
+  <si>
+    <t>x0001FF</t>
+  </si>
+  <si>
+    <t>if LSB=0, ext trig input acts as 'gate only' for scalers</t>
+  </si>
+  <si>
+    <t>(0) : accept external trig input to data manager; (1) : use gate generator; (8-23) : gate generator width</t>
+  </si>
+  <si>
+    <t>x00FF00</t>
+  </si>
+  <si>
+    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; replace trigger output with 1Hz heartbeat pulse (debug use only) ; bits 8 to 15-&gt;width as specified by 25 MHz clock cycles</t>
+  </si>
+  <si>
+    <t>update scalers + ext trig latched timestamp</t>
+  </si>
+  <si>
+    <t>write a 1 to LSB to save scaler values and update latched timestamp value</t>
+  </si>
+  <si>
+    <t>latched_timestamp low 24 bits</t>
+  </si>
+  <si>
+    <t>latched_timestamp high 24 bits</t>
+  </si>
+  <si>
+    <t>running timestamp saved on ext trig input (i.e. PPS)</t>
+  </si>
+  <si>
+    <t>update register by writing LSB in reg 40</t>
   </si>
 </sst>
 </file>
@@ -786,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -849,8 +873,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1133,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,38 +1177,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="37">
         <v>42917</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>74</v>
@@ -1200,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1223,10 +1251,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1271,13 +1299,13 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,7 +1324,7 @@
         <v>73</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1328,13 +1356,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1353,7 +1381,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1366,13 +1394,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1385,7 +1413,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1401,16 +1429,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1423,10 +1451,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>7</v>
@@ -1443,10 +1471,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>7</v>
@@ -1463,10 +1491,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>7</v>
@@ -1483,10 +1511,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>7</v>
@@ -1503,10 +1531,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>7</v>
@@ -1523,16 +1551,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1545,16 +1573,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1567,16 +1595,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>98</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1589,10 +1617,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>7</v>
@@ -1609,7 +1637,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1629,7 +1657,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1649,7 +1677,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1669,7 +1697,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1689,7 +1717,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1709,7 +1737,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1729,7 +1757,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1749,7 +1777,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1769,7 +1797,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1789,7 +1817,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1809,7 +1837,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1829,7 +1857,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1849,7 +1877,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1869,7 +1897,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1889,7 +1917,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1909,13 +1937,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,13 +1956,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" s="25" t="s">
         <v>129</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="F43" s="25" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,13 +1975,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1966,13 +1994,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="D45" s="24" t="s">
-        <v>134</v>
-      </c>
       <c r="F45" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1985,16 +2013,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2007,10 +2035,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>208</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2026,16 +2054,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="D48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2079,6 +2107,15 @@
         <f t="shared" si="0"/>
         <v>x2C</v>
       </c>
+      <c r="C51" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" t="s">
+        <v>213</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -2089,6 +2126,15 @@
         <f t="shared" si="0"/>
         <v>x2D</v>
       </c>
+      <c r="C52" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2129,7 +2175,7 @@
         <v>80</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2161,7 +2207,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2183,7 +2229,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2205,7 +2251,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2269,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2288,7 +2334,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2307,7 +2353,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2326,7 +2372,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2351,7 +2397,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2416,7 +2462,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2479,13 +2525,13 @@
         <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2518,7 +2564,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2540,7 +2586,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2563,9 +2609,11 @@
         <f t="shared" si="2"/>
         <v>x4A</v>
       </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="13"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -2574,7 +2622,18 @@
         <f t="shared" si="2"/>
         <v>x4B</v>
       </c>
-      <c r="F82" s="11"/>
+      <c r="C82" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F82" s="39" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83">
@@ -2592,10 +2651,10 @@
         <v>72</v>
       </c>
       <c r="E83" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2608,16 +2667,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D84" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2639,7 +2698,7 @@
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2671,7 +2730,7 @@
         <v>70</v>
       </c>
       <c r="E87" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>69</v>
@@ -2687,19 +2746,19 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E88" t="s">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -2709,16 +2768,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
       <c r="E89" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2731,16 +2790,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="E90" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2753,16 +2812,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D91" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2775,10 +2834,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
@@ -2803,7 +2862,7 @@
         <v>64</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3111,10 +3170,10 @@
         <v>x67</v>
       </c>
       <c r="C110" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3127,7 +3186,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3140,7 +3199,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="33" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3153,7 +3212,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="34" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3166,7 +3225,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="34" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3179,16 +3238,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E115" s="32" t="s">
         <v>7</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3201,7 +3260,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3210,7 +3269,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3223,10 +3282,10 @@
         <v>x6E</v>
       </c>
       <c r="C117" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D117" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3239,10 +3298,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D118" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3255,10 +3314,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D119" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3271,10 +3330,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="33" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3287,10 +3346,10 @@
         <v>x72</v>
       </c>
       <c r="C121" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D121" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3303,10 +3362,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3319,10 +3378,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="33" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3335,10 +3394,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="33" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D124" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3351,10 +3410,10 @@
         <v>x76</v>
       </c>
       <c r="C125" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3367,10 +3426,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="33" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,7 +3442,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="34" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3396,10 +3455,10 @@
         <v>x79</v>
       </c>
       <c r="C128" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D128" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3435,13 +3494,13 @@
         <v>35</v>
       </c>
       <c r="D131" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F131" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="E131" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F131" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3464,10 +3523,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D133" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3486,7 +3545,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
South Pole updates / as deployed Jan 2018
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\firmware-phased-array\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\firmware\firmware-phased-array\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26730" windowHeight="9585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13584" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -671,7 +671,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1161,22 +1161,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="4" width="82.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="6" width="74.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="E3" s="37"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>42917</v>
       </c>
@@ -1217,13 +1217,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>1+A8</f>
         <v>2</v>
@@ -1289,7 +1289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" ref="A10:A73" si="1">1+A9</f>
         <v>3</v>
@@ -1308,7 +1308,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1327,7 +1327,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1346,7 +1346,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1365,7 +1365,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1384,7 +1384,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1403,7 +1403,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1419,7 +1419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1441,7 +1441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1563,7 +1563,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1585,7 +1585,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1607,7 +1607,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="18">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="F32" s="20"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="18">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="F35" s="20"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="18">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="F37" s="20"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="18">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="F40" s="20"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="21">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="F41" s="23"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1946,7 +1946,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1965,7 +1965,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -1984,7 +1984,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -2003,7 +2003,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -2025,7 +2025,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2044,7 +2044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2066,7 +2066,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2088,7 +2088,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2098,7 +2098,7 @@
         <v>x2B</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -2117,7 +2117,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -2136,7 +2136,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -2146,7 +2146,7 @@
         <v>x2E</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -2156,7 +2156,7 @@
         <v>x2F</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2178,7 +2178,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -2188,7 +2188,7 @@
         <v>x31</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -2210,7 +2210,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2232,7 +2232,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2254,7 +2254,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2273,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2283,7 +2283,7 @@
         <v>x36</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2302,7 +2302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2321,7 +2321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2340,7 +2340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2359,7 +2359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -2378,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2400,7 +2400,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2410,7 +2410,7 @@
         <v>x3D</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2420,7 +2420,7 @@
         <v>x3E</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2430,7 +2430,7 @@
         <v>x3F</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2449,7 +2449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -2468,7 +2468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -2490,7 +2490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="9">
         <f t="shared" ref="A74:A134" si="3">1+A73</f>
         <v>67</v>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="F74" s="11"/>
     </row>
-    <row r="75" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="9">
         <f t="shared" si="3"/>
         <v>68</v>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="F75" s="11"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="9">
         <f t="shared" si="3"/>
         <v>69</v>
@@ -2534,7 +2534,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="9">
         <f t="shared" si="3"/>
         <v>70</v>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="9">
         <f t="shared" si="3"/>
         <v>71</v>
@@ -2567,7 +2567,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <f t="shared" si="3"/>
         <v>72</v>
@@ -2589,7 +2589,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="9">
         <f t="shared" si="3"/>
         <v>73</v>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="9">
         <f t="shared" si="3"/>
         <v>74</v>
@@ -2613,7 +2613,7 @@
       <c r="D81" s="13"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="9">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -2635,7 +2635,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="3"/>
         <v>76</v>
@@ -2657,7 +2657,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -2679,7 +2679,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="3"/>
         <v>78</v>
@@ -2701,7 +2701,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="3"/>
         <v>79</v>
@@ -2714,7 +2714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="3"/>
         <v>80</v>
@@ -2736,7 +2736,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="3"/>
         <v>81</v>
@@ -2758,7 +2758,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="3"/>
         <v>82</v>
@@ -2780,7 +2780,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="3"/>
         <v>83</v>
@@ -2802,7 +2802,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>84</v>
@@ -2824,7 +2824,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -2843,7 +2843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -2865,7 +2865,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -2884,7 +2884,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -2903,7 +2903,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -2922,7 +2922,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -2941,7 +2941,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -2960,7 +2960,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -2979,7 +2979,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>93</v>
@@ -2998,7 +2998,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>94</v>
@@ -3017,7 +3017,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -3036,7 +3036,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>96</v>
@@ -3055,7 +3055,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -3074,7 +3074,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -3093,7 +3093,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -3112,7 +3112,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -3131,7 +3131,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -3150,7 +3150,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -3160,7 +3160,7 @@
         <v>x66</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -3176,7 +3176,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -3189,7 +3189,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -3202,7 +3202,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -3215,7 +3215,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -3228,7 +3228,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -3250,7 +3250,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -3272,7 +3272,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -3288,7 +3288,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -3304,7 +3304,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <f t="shared" si="3"/>
         <v>112</v>
@@ -3320,7 +3320,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -3336,7 +3336,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -3352,7 +3352,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -3368,7 +3368,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -3384,7 +3384,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -3400,7 +3400,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -3416,7 +3416,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -3432,7 +3432,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>120</v>
@@ -3445,7 +3445,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -3461,7 +3461,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -3471,7 +3471,7 @@
         <v>x7A</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -3481,7 +3481,7 @@
         <v>x7B</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -3503,7 +3503,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -3513,7 +3513,7 @@
         <v>x7D</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -3532,7 +3532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>127</v>

</xml_diff>

<commit_message>
reduce FIFO pipeline length, add gate flag to metadata
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -317,9 +317,6 @@
     <t>metadata-&gt;unassigned</t>
   </si>
   <si>
-    <t>bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
-  </si>
-  <si>
     <t>bit0-&gt;global reset, bit1-&gt;reset global EXCEPT register settings, bit2-&gt;reset ADC (restart+cal cycle)</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
   </si>
   <si>
     <t>lower three bits used, set value to 0 thru 7. Pretrig window set to value*8*10.66ns</t>
+  </si>
+  <si>
+    <t>bit 23 : gate flag ; bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1251,10 +1251,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1305,7 +1305,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
         <v>72</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,13 +1356,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1394,13 +1394,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1413,7 +1413,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1560,7 +1560,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>85</v>
@@ -1582,7 +1582,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1657,7 +1657,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1677,7 +1677,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1697,7 +1697,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1717,7 +1717,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1737,7 +1737,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1757,7 +1757,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1777,7 +1777,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1797,7 +1797,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1817,7 +1817,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1837,7 +1837,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1857,7 +1857,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1877,7 +1877,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1897,7 +1897,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1917,7 +1917,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1937,13 +1937,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,13 +1956,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1975,13 +1975,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1994,13 +1994,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2013,16 +2013,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2035,10 +2035,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
+        <v>206</v>
+      </c>
+      <c r="D47" t="s">
         <v>207</v>
-      </c>
-      <c r="D47" t="s">
-        <v>208</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2108,13 +2108,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,13 +2127,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="D52" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,7 +2175,7 @@
         <v>79</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2334,7 +2334,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2353,7 +2353,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2372,7 +2372,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2397,7 +2397,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2525,13 +2525,13 @@
         <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2623,16 +2623,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D82" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="E82" s="9" t="s">
-        <v>205</v>
-      </c>
       <c r="F82" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2648,13 +2648,13 @@
         <v>71</v>
       </c>
       <c r="D83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E83" t="s">
+        <v>161</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2667,16 +2667,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>148</v>
+      </c>
+      <c r="D84" t="s">
         <v>149</v>
-      </c>
-      <c r="D84" t="s">
-        <v>150</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2698,7 +2698,7 @@
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2730,7 +2730,7 @@
         <v>70</v>
       </c>
       <c r="E87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>69</v>
@@ -2746,16 +2746,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E88" t="s">
+        <v>201</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="E88" t="s">
-        <v>202</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2768,16 +2768,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
+        <v>197</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>199</v>
-      </c>
       <c r="E89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2790,16 +2790,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
+        <v>140</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E90" t="s">
+        <v>142</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="E90" t="s">
-        <v>143</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2812,16 +2812,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>153</v>
+      </c>
+      <c r="D91" t="s">
         <v>154</v>
-      </c>
-      <c r="D91" t="s">
-        <v>155</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2834,10 +2834,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>171</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
@@ -2862,7 +2862,7 @@
         <v>64</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3170,10 +3170,10 @@
         <v>x67</v>
       </c>
       <c r="C110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D110" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3186,7 +3186,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,7 +3199,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3212,7 +3212,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3225,7 +3225,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3238,16 +3238,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="D115" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="E115" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3269,7 +3269,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3282,10 +3282,10 @@
         <v>x6E</v>
       </c>
       <c r="C117" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D117" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3298,10 +3298,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D118" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3314,10 +3314,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D119" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3330,10 +3330,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3346,10 +3346,10 @@
         <v>x72</v>
       </c>
       <c r="C121" t="s">
+        <v>182</v>
+      </c>
+      <c r="D121" t="s">
         <v>183</v>
-      </c>
-      <c r="D121" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3362,10 +3362,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3378,10 +3378,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3394,10 +3394,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D124" t="s">
         <v>185</v>
-      </c>
-      <c r="D124" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3410,10 +3410,10 @@
         <v>x76</v>
       </c>
       <c r="C125" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3426,10 +3426,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3455,10 +3455,10 @@
         <v>x79</v>
       </c>
       <c r="C128" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D128" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3494,13 +3494,13 @@
         <v>35</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3545,7 +3545,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
reduce trig out latency, uptick version to 1.12
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="215">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -449,9 +449,6 @@
     <t>external trigger output config</t>
   </si>
   <si>
-    <t>default width of 120 ns</t>
-  </si>
-  <si>
     <t>x000303</t>
   </si>
   <si>
@@ -641,9 +638,6 @@
     <t>x00FF00</t>
   </si>
   <si>
-    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; replace trigger output with 1Hz heartbeat pulse (debug use only) ; bits 8 to 15-&gt;width as specified by 25 MHz clock cycles</t>
-  </si>
-  <si>
     <t>update scalers + ext trig latched timestamp</t>
   </si>
   <si>
@@ -666,6 +660,15 @@
   </si>
   <si>
     <t>bit 23 : gate flag ; bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
+  </si>
+  <si>
+    <t>bit 0-&gt;enable; bit1-&gt;polarity; bit2-&gt; replace trigger output with 1Hz heartbeat pulse (debug use only) ; bits 8 to 15-&gt;width as specified by *93* MHz clock cycles</t>
+  </si>
+  <si>
+    <t>default width of 128 ns [note: update on 2/20/18 put output trig on 93.75 MHz clock, instead of 25 Mhz clock]</t>
+  </si>
+  <si>
+    <t>x000C03</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1308,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,13 +1359,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1560,7 +1563,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1604,7 +1607,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2013,16 +2016,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2035,10 +2038,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2108,13 +2111,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
+        <v>206</v>
+      </c>
+      <c r="D51" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D51" t="s">
-        <v>211</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,13 +2130,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="D52" s="35" t="s">
-        <v>211</v>
-      </c>
       <c r="F52" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,7 +2178,7 @@
         <v>79</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2207,7 +2210,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,7 +2232,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2251,7 +2254,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,7 +2318,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2334,7 +2337,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2353,7 +2356,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2372,7 +2375,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2397,7 +2400,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2623,16 +2626,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D82" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E82" s="9" t="s">
-        <v>204</v>
-      </c>
       <c r="F82" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2648,13 +2651,13 @@
         <v>71</v>
       </c>
       <c r="D83" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E83" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2667,16 +2670,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>147</v>
+      </c>
+      <c r="D84" t="s">
         <v>148</v>
-      </c>
-      <c r="D84" t="s">
-        <v>149</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2749,13 +2752,13 @@
         <v>98</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E88" t="s">
+        <v>200</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="E88" t="s">
-        <v>201</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2768,16 +2771,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
+        <v>196</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>198</v>
-      </c>
       <c r="E89" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2793,13 +2796,13 @@
         <v>140</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E90" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>141</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2812,16 +2815,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>152</v>
+      </c>
+      <c r="D91" t="s">
         <v>153</v>
-      </c>
-      <c r="D91" t="s">
-        <v>154</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2834,10 +2837,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
@@ -3170,10 +3173,10 @@
         <v>x67</v>
       </c>
       <c r="C110" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D110" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3186,7 +3189,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,7 +3202,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3212,7 +3215,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3225,7 +3228,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3238,16 +3241,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="D115" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="E115" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3282,10 +3285,10 @@
         <v>x6E</v>
       </c>
       <c r="C117" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3298,10 +3301,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D118" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3314,10 +3317,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D119" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3330,10 +3333,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3346,10 +3349,10 @@
         <v>x72</v>
       </c>
       <c r="C121" t="s">
+        <v>181</v>
+      </c>
+      <c r="D121" t="s">
         <v>182</v>
-      </c>
-      <c r="D121" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3362,10 +3365,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3378,10 +3381,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3394,10 +3397,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="D124" t="s">
         <v>184</v>
-      </c>
-      <c r="D124" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3410,10 +3413,10 @@
         <v>x76</v>
       </c>
       <c r="C125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3426,10 +3429,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3442,7 +3445,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3455,10 +3458,10 @@
         <v>x79</v>
       </c>
       <c r="C128" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D128" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3494,13 +3497,13 @@
         <v>35</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update beamformer: include channel-specific programmable sample delays
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -449,9 +449,6 @@
     <t>external trigger output config</t>
   </si>
   <si>
-    <t>x000303</t>
-  </si>
-  <si>
     <t>sync command</t>
   </si>
   <si>
@@ -669,6 +666,21 @@
   </si>
   <si>
     <t>x000C03</t>
+  </si>
+  <si>
+    <t>trig delay: CH's 0,1,2</t>
+  </si>
+  <si>
+    <t>trig delay: CH's 3,4,5</t>
+  </si>
+  <si>
+    <t>trig delay: CH's 6,7</t>
+  </si>
+  <si>
+    <t>one byte each channel</t>
+  </si>
+  <si>
+    <t>note channel 5 hard-coded masked from trigger (dead vpol channel)</t>
   </si>
 </sst>
 </file>
@@ -813,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -879,6 +891,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1164,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,38 +1193,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
+      <c r="A4" s="39">
         <v>42917</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>73</v>
@@ -1308,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,13 +1372,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1563,7 +1576,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1607,7 +1620,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2016,16 +2029,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2038,10 +2051,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" t="s">
         <v>204</v>
-      </c>
-      <c r="D47" t="s">
-        <v>205</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2111,13 +2124,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2130,13 +2143,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="D52" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,7 +2191,7 @@
         <v>79</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2210,7 +2223,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2232,7 +2245,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2318,7 +2331,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2337,7 +2350,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2356,7 +2369,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2375,7 +2388,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2400,7 +2413,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2412,6 +2425,12 @@
         <f t="shared" si="0"/>
         <v>x3D</v>
       </c>
+      <c r="C68" t="s">
+        <v>214</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
@@ -2422,6 +2441,15 @@
         <f t="shared" si="0"/>
         <v>x3E</v>
       </c>
+      <c r="C69" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -2431,6 +2459,12 @@
       <c r="B70" s="28" t="str">
         <f t="shared" si="0"/>
         <v>x3F</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2626,16 +2660,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D82" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E82" s="9" t="s">
-        <v>203</v>
-      </c>
       <c r="F82" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2651,13 +2685,13 @@
         <v>71</v>
       </c>
       <c r="D83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E83" t="s">
+        <v>159</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,16 +2704,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" t="s">
         <v>147</v>
-      </c>
-      <c r="D84" t="s">
-        <v>148</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2752,13 +2786,13 @@
         <v>98</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E88" t="s">
+        <v>199</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="E88" t="s">
-        <v>200</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2771,16 +2805,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
+        <v>195</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="E89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2796,13 +2830,13 @@
         <v>140</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E90" t="s">
+        <v>213</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="E90" t="s">
-        <v>214</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2815,16 +2849,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" t="s">
         <v>152</v>
-      </c>
-      <c r="D91" t="s">
-        <v>153</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2837,10 +2871,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>169</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
@@ -3173,10 +3207,10 @@
         <v>x67</v>
       </c>
       <c r="C110" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,7 +3223,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3202,7 +3236,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,7 +3249,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,7 +3262,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3241,16 +3275,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="D115" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="E115" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,10 +3319,10 @@
         <v>x6E</v>
       </c>
       <c r="C117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D117" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3301,10 +3335,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D118" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3317,10 +3351,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D119" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3333,10 +3367,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3349,10 +3383,10 @@
         <v>x72</v>
       </c>
       <c r="C121" t="s">
+        <v>180</v>
+      </c>
+      <c r="D121" t="s">
         <v>181</v>
-      </c>
-      <c r="D121" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3365,10 +3399,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3381,10 +3415,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3397,10 +3431,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D124" t="s">
         <v>183</v>
-      </c>
-      <c r="D124" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3413,10 +3447,10 @@
         <v>x76</v>
       </c>
       <c r="C125" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3429,10 +3463,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3445,7 +3479,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3458,10 +3492,10 @@
         <v>x79</v>
       </c>
       <c r="C128" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D128" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3497,13 +3531,13 @@
         <v>35</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working towards surface trigger
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="221">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -681,6 +681,12 @@
   </si>
   <si>
     <t>note channel 5 hard-coded masked from trigger (dead vpol channel)</t>
+  </si>
+  <si>
+    <t>surface trigger..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower byte = vpp_Threshold ; </t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,6 +2167,12 @@
         <f t="shared" si="0"/>
         <v>x2E</v>
       </c>
+      <c r="C53" t="s">
+        <v>219</v>
+      </c>
+      <c r="D53" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">

</xml_diff>

<commit_message>
compiled surface trigger module on slave board
also add functionality for powering down surface ADCs (for temp concerns
within the box)
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="225">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -686,7 +686,19 @@
     <t>surface trigger..</t>
   </si>
   <si>
-    <t xml:space="preserve">lower byte = vpp_Threshold ; </t>
+    <t>surface trigger2..</t>
+  </si>
+  <si>
+    <t>bits(2-0) = min number channels, bit 8 = select surface readout, bit 16 enable surface ADCs and surface trigger</t>
+  </si>
+  <si>
+    <t>lower byte = vpp_Threshold ; middle byte = trig window length ; high byte = 'mask' (1=enable)</t>
+  </si>
+  <si>
+    <t>0x380914</t>
+  </si>
+  <si>
+    <t>0x010002</t>
   </si>
 </sst>
 </file>
@@ -1183,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1204,7 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="14" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.85546875" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>
@@ -2171,17 +2183,29 @@
         <v>219</v>
       </c>
       <c r="D53" t="s">
+        <v>222</v>
+      </c>
+      <c r="E53" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B54" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>x2F</v>
+      </c>
+      <c r="C54" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="B54" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>x2F</v>
+      <c r="D54" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E54" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add separate buffer clear for surface event storage
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -467,9 +467,6 @@
     <t>rdout-&gt;clear  buffer full, set buffer num to zero</t>
   </si>
   <si>
-    <t>lower four bits clear each of the 4 event buffers, bit 8 sets buffer to 0</t>
-  </si>
-  <si>
     <t>functionality to reset buffer to zero only works if not currently saving an event.</t>
   </si>
   <si>
@@ -699,6 +696,9 @@
   </si>
   <si>
     <t>0x010002</t>
+  </si>
+  <si>
+    <t>lower four bits clear each of the 4 event buffers, bit 8 sets buffer to 0, bit 16 is buffer clear for surface event buffer</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1339,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,13 +1390,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2069,10 +2069,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" t="s">
         <v>203</v>
-      </c>
-      <c r="D47" t="s">
-        <v>204</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2142,13 +2142,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2161,13 +2161,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="D52" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2180,13 +2180,13 @@
         <v>x2E</v>
       </c>
       <c r="C53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D53" t="s">
+        <v>221</v>
+      </c>
+      <c r="E53" t="s">
         <v>222</v>
-      </c>
-      <c r="E53" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2199,13 +2199,13 @@
         <v>x2F</v>
       </c>
       <c r="C54" t="s">
+        <v>219</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>221</v>
-      </c>
       <c r="E54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>79</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,7 +2259,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2303,7 +2303,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2386,7 +2386,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2405,7 +2405,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2424,7 +2424,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2449,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,10 +2462,10 @@
         <v>x3D</v>
       </c>
       <c r="C68" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2478,13 +2478,13 @@
         <v>x3E</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D69" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,10 +2497,10 @@
         <v>x3F</v>
       </c>
       <c r="C70" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2696,16 +2696,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D82" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E82" s="9" t="s">
-        <v>202</v>
-      </c>
       <c r="F82" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2720,17 +2720,17 @@
       <c r="C83" t="s">
         <v>71</v>
       </c>
-      <c r="D83" t="s">
-        <v>209</v>
+      <c r="D83" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="E83" t="s">
+        <v>158</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F83" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="3"/>
         <v>77</v>
@@ -2742,14 +2742,14 @@
       <c r="C84" t="s">
         <v>146</v>
       </c>
-      <c r="D84" t="s">
-        <v>147</v>
+      <c r="D84" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
       <c r="C85" t="s">
         <v>75</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E85" t="s">
@@ -2783,7 +2783,7 @@
         <f t="shared" si="2"/>
         <v>x4F</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2799,7 +2799,7 @@
       <c r="C87" t="s">
         <v>68</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E87" t="s">
@@ -2822,13 +2822,13 @@
         <v>98</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E88" t="s">
+        <v>198</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="E88" t="s">
-        <v>199</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,13 +2841,13 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
+        <v>194</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="E89" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>144</v>
@@ -2866,13 +2866,13 @@
         <v>140</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E90" t="s">
+        <v>212</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="E90" t="s">
-        <v>213</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2885,16 +2885,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
+        <v>150</v>
+      </c>
+      <c r="D91" t="s">
         <v>151</v>
-      </c>
-      <c r="D91" t="s">
-        <v>152</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2907,10 +2907,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
+        <v>168</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
@@ -3243,10 +3243,10 @@
         <v>x67</v>
       </c>
       <c r="C110" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D110" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,7 +3272,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3298,7 +3298,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3311,16 +3311,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="D115" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="E115" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3355,10 +3355,10 @@
         <v>x6E</v>
       </c>
       <c r="C117" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D117" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3371,10 +3371,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D118" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3387,10 +3387,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D119" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3403,10 +3403,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3419,10 +3419,10 @@
         <v>x72</v>
       </c>
       <c r="C121" t="s">
+        <v>179</v>
+      </c>
+      <c r="D121" t="s">
         <v>180</v>
-      </c>
-      <c r="D121" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3435,10 +3435,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3451,10 +3451,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3467,10 +3467,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D124" t="s">
         <v>182</v>
-      </c>
-      <c r="D124" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3483,10 +3483,10 @@
         <v>x76</v>
       </c>
       <c r="C125" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3499,10 +3499,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3528,10 +3528,10 @@
         <v>x79</v>
       </c>
       <c r="C128" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D128" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3567,13 +3567,13 @@
         <v>35</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
anoter surface trig update
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -224,12 +225,6 @@
     <t>threshold for calculated power in beam</t>
   </si>
   <si>
-    <t>bits 0 and 1 select readout type (register [0], wfm [1], beams[2], powsum[3])</t>
-  </si>
-  <si>
-    <t>also pick between beam8, beam4a, beam4b using bits 2 and 3 (0,1,2)</t>
-  </si>
-  <si>
     <t>trigger mask</t>
   </si>
   <si>
@@ -428,9 +423,6 @@
     <t>bits 3 to 0 -&gt; 1 indicates each ADCs locked datastream ; bits 11 to 8-&gt;ADC pd ; bit 16-&gt; adc startup signal</t>
   </si>
   <si>
-    <t>bits 3 to 0-&gt;buffer full flags; bit 8-&gt;OR of buffer full flags; bits 13 to 12-&gt;next_buffer ; bits 17 to 16-&gt; last trig type</t>
-  </si>
-  <si>
     <t>NO FUNCTION</t>
   </si>
   <si>
@@ -500,12 +492,6 @@
     <t>block/allow channels in beam-forming</t>
   </si>
   <si>
-    <t>x000004</t>
-  </si>
-  <si>
-    <t>Default updated 9/1/2017 and tested: puts triggered pulse at beginning of readout window</t>
-  </si>
-  <si>
     <t>chip_id(high) + fpga temperature</t>
   </si>
   <si>
@@ -650,9 +636,6 @@
     <t>update register by writing LSB in reg 40</t>
   </si>
   <si>
-    <t>lower three bits used, set value to 0 thru 7. Pretrig window set to value*8*10.66ns</t>
-  </si>
-  <si>
     <t>bit 23 : gate flag ; bits 22-15 : channel mask ; bits 14-0 : beam mask</t>
   </si>
   <si>
@@ -699,6 +682,24 @@
   </si>
   <si>
     <t>lower four bits clear each of the 4 event buffers, bit 8 sets buffer to 0, bit 16 is buffer clear for surface event buffer</t>
+  </si>
+  <si>
+    <t>lower three bits used, set value to 0 thru 7. Pretrig window set to value*8*10.66ns. Middle byte for surface array</t>
+  </si>
+  <si>
+    <t>x000404</t>
+  </si>
+  <si>
+    <t>Default updated 9/1/2017 and tested: puts triggered pulse at beginning of readout window. Surface stuff added 1/15/2019</t>
+  </si>
+  <si>
+    <t>bits 3 to 0-&gt;buffer full flags; bit 4-&gt;surface buffer full (slave board only); bit 8-&gt;OR of buffer full flags; bits 13 to 12-&gt;next_buffer ; bits 17 to 16-&gt; last trig type</t>
+  </si>
+  <si>
+    <t>bits 0 and 1 select readout type (register [0], wfm [1)</t>
+  </si>
+  <si>
+    <t>looks to be an unused register 1/16/2019</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1246,7 @@
       <c r="B4" s="40"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
@@ -1262,7 +1263,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1285,10 +1286,10 @@
         <v>x00</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1333,13 +1334,13 @@
         <v>x03</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,10 +1356,10 @@
         <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1374,7 +1375,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>41</v>
@@ -1390,13 +1391,13 @@
         <v>x06</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1409,13 +1410,13 @@
         <v>x07</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>134</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1428,13 +1429,13 @@
         <v>x08</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1447,7 +1448,7 @@
         <v>x09</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -1463,16 +1464,16 @@
         <v>x0A</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,10 +1486,10 @@
         <v>x0B</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>7</v>
@@ -1505,10 +1506,10 @@
         <v>x0C</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>7</v>
@@ -1525,10 +1526,10 @@
         <v>x0D</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>7</v>
@@ -1545,10 +1546,10 @@
         <v>x0E</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>7</v>
@@ -1565,10 +1566,10 @@
         <v>x0F</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>7</v>
@@ -1585,16 +1586,16 @@
         <v>x10</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1607,16 +1608,16 @@
         <v>x11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1629,16 +1630,16 @@
         <v>x12</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1651,10 +1652,10 @@
         <v>x13</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>7</v>
@@ -1671,7 +1672,7 @@
         <v>x14</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>17</v>
@@ -1691,7 +1692,7 @@
         <v>x15</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>17</v>
@@ -1711,7 +1712,7 @@
         <v>x16</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>17</v>
@@ -1731,7 +1732,7 @@
         <v>x17</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>17</v>
@@ -1751,7 +1752,7 @@
         <v>x18</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>17</v>
@@ -1771,7 +1772,7 @@
         <v>x19</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>17</v>
@@ -1791,7 +1792,7 @@
         <v>x1A</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>17</v>
@@ -1811,7 +1812,7 @@
         <v>x1B</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>17</v>
@@ -1831,7 +1832,7 @@
         <v>x1C</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>17</v>
@@ -1851,7 +1852,7 @@
         <v>x1D</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>17</v>
@@ -1871,7 +1872,7 @@
         <v>x1E</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>17</v>
@@ -1891,7 +1892,7 @@
         <v>x1F</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>17</v>
@@ -1911,7 +1912,7 @@
         <v>x20</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>17</v>
@@ -1931,7 +1932,7 @@
         <v>x21</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
@@ -1951,7 +1952,7 @@
         <v>x22</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>17</v>
@@ -1971,13 +1972,13 @@
         <v>x23</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1990,13 +1991,13 @@
         <v>x24</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2009,13 +2010,13 @@
         <v>x25</v>
       </c>
       <c r="C44" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="25" t="s">
         <v>125</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,13 +2029,13 @@
         <v>x26</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2047,16 +2048,16 @@
         <v>x27</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E46" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2069,10 +2070,10 @@
         <v>x28</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D47" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -2088,16 +2089,16 @@
         <v>x29</v>
       </c>
       <c r="C48" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D48" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2142,13 +2143,13 @@
         <v>x2C</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D51" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2161,13 +2162,13 @@
         <v>x2D</v>
       </c>
       <c r="C52" s="35" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2180,13 +2181,13 @@
         <v>x2E</v>
       </c>
       <c r="C53" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D53" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E53" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2199,13 +2200,13 @@
         <v>x2F</v>
       </c>
       <c r="C54" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E54" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2221,13 +2222,13 @@
         <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,7 +2260,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2281,7 +2282,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2303,7 +2304,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,7 +2349,7 @@
         <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
@@ -2367,7 +2368,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>7</v>
@@ -2386,7 +2387,7 @@
         <v>31</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>7</v>
@@ -2405,7 +2406,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
@@ -2424,7 +2425,7 @@
         <v>33</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>7</v>
@@ -2449,7 +2450,7 @@
         <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,10 +2463,10 @@
         <v>x3D</v>
       </c>
       <c r="C68" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2478,13 +2479,13 @@
         <v>x3E</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,10 +2498,10 @@
         <v>x3F</v>
       </c>
       <c r="C70" s="37" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2535,7 +2536,7 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2554,13 +2555,13 @@
         <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>66</v>
+        <v>223</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>67</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2598,13 +2599,13 @@
         <v>36</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2637,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2659,7 +2660,7 @@
         <v>8</v>
       </c>
       <c r="F79" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2696,16 +2697,16 @@
         <v>x4B</v>
       </c>
       <c r="C82" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D82" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>201</v>
-      </c>
       <c r="F82" s="36" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2718,16 +2719,16 @@
         <v>x4C</v>
       </c>
       <c r="C83" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="E83" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>159</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2740,16 +2741,16 @@
         <v>x4D</v>
       </c>
       <c r="C84" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2762,16 +2763,16 @@
         <v>x4E</v>
       </c>
       <c r="C85" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2797,16 +2798,16 @@
         <v>x50</v>
       </c>
       <c r="C87" t="s">
+        <v>66</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D87" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="E87" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2819,16 +2820,16 @@
         <v>x51</v>
       </c>
       <c r="C88" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E88" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,16 +2842,16 @@
         <v>x52</v>
       </c>
       <c r="C89" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E89" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2863,16 +2864,16 @@
         <v>x53</v>
       </c>
       <c r="C90" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E90" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2885,16 +2886,16 @@
         <v>x54</v>
       </c>
       <c r="C91" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D91" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2907,10 +2908,10 @@
         <v>x55</v>
       </c>
       <c r="C92" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>12</v>
@@ -2935,7 +2936,7 @@
         <v>64</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3243,10 +3244,10 @@
         <v>x67</v>
       </c>
       <c r="C110" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D110" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,7 +3260,7 @@
         <v>x68</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,7 +3273,7 @@
         <v>x69</v>
       </c>
       <c r="C112" s="33" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3285,7 +3286,7 @@
         <v>x6A</v>
       </c>
       <c r="C113" s="34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3298,7 +3299,7 @@
         <v>x6B</v>
       </c>
       <c r="C114" s="34" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3311,16 +3312,16 @@
         <v>x6C</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E115" s="32" t="s">
         <v>7</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3333,7 +3334,7 @@
         <v>x6D</v>
       </c>
       <c r="C116" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D116" t="s">
         <v>19</v>
@@ -3342,7 +3343,7 @@
         <v>20</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3355,10 +3356,10 @@
         <v>x6E</v>
       </c>
       <c r="C117" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D117" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3371,10 +3372,10 @@
         <v>x6F</v>
       </c>
       <c r="C118" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D118" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3387,10 +3388,10 @@
         <v>x70</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D119" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3403,10 +3404,10 @@
         <v>x71</v>
       </c>
       <c r="C120" s="33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3419,10 +3420,10 @@
         <v>x72</v>
       </c>
       <c r="C121" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D121" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3435,10 +3436,10 @@
         <v>x73</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3451,10 +3452,10 @@
         <v>x74</v>
       </c>
       <c r="C123" s="33" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3467,10 +3468,10 @@
         <v>x75</v>
       </c>
       <c r="C124" s="33" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D124" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3483,10 +3484,10 @@
         <v>x76</v>
       </c>
       <c r="C125" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3499,10 +3500,10 @@
         <v>x77</v>
       </c>
       <c r="C126" s="33" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3515,7 +3516,7 @@
         <v>x78</v>
       </c>
       <c r="C127" s="34" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3528,10 +3529,10 @@
         <v>x79</v>
       </c>
       <c r="C128" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D128" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3567,13 +3568,13 @@
         <v>35</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3596,10 +3597,10 @@
         <v>x7E</v>
       </c>
       <c r="C133" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D133" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3618,7 +3619,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add polarization cut on surface trigger
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="226">
   <si>
     <t>Firmware-phased-array</t>
   </si>
@@ -669,9 +669,6 @@
     <t>surface trigger2..</t>
   </si>
   <si>
-    <t>bits(2-0) = min number channels, bit 8 = select surface readout, bit 16 enable surface ADCs and surface trigger</t>
-  </si>
-  <si>
     <t>lower byte = vpp_Threshold ; middle byte = trig window length ; high byte = 'mask' (1=enable)</t>
   </si>
   <si>
@@ -700,6 +697,12 @@
   </si>
   <si>
     <t>looks to be an unused register 1/16/2019</t>
+  </si>
+  <si>
+    <t>bits(2-0) = min number channels, bit 4=require Hpol&gt;Vpol, bit 5 bit 8 = select surface readout, bit 16 enable surface ADCs and surface trigger</t>
+  </si>
+  <si>
+    <t>Hpol Surface Power threshold</t>
   </si>
 </sst>
 </file>
@@ -844,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -910,6 +913,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -1196,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,38 +1216,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
+      <c r="A4" s="40">
         <v>42917</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>71</v>
@@ -1416,7 +1420,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2184,10 +2188,10 @@
         <v>212</v>
       </c>
       <c r="D53" t="s">
+        <v>214</v>
+      </c>
+      <c r="E53" t="s">
         <v>215</v>
-      </c>
-      <c r="E53" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2203,10 +2207,10 @@
         <v>213</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="E54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2555,13 +2559,13 @@
         <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2722,13 +2726,13 @@
         <v>69</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E83" t="s">
         <v>219</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2744,7 +2748,7 @@
         <v>143</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -3232,6 +3236,12 @@
       <c r="B109" s="28" t="str">
         <f t="shared" si="2"/>
         <v>x66</v>
+      </c>
+      <c r="C109" t="s">
+        <v>225</v>
+      </c>
+      <c r="E109" s="38" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update doc for surface changes
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\firmware-phased-array\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\firmware-phased-array\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4E3279-4343-41DE-A41F-9AEA3829404E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="5775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -699,16 +704,16 @@
     <t>looks to be an unused register 1/16/2019</t>
   </si>
   <si>
-    <t>bits(2-0) = min number channels, bit 4=require Hpol&gt;Vpol, bit 5 bit 8 = select surface readout, bit 16 enable surface ADCs and surface trigger</t>
-  </si>
-  <si>
     <t>Hpol Surface Power threshold</t>
+  </si>
+  <si>
+    <t>bits(2-0) = min number channels, bit 3 FIR high pass enable, bit 4=require Hpol&gt;Vpol, bit 5 bit 8 = select surface readout, bit 16 enable surface ADCs and surface trigger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1197,11 +1202,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,7 +2212,7 @@
         <v>213</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E54" t="s">
         <v>216</v>
@@ -3238,7 +3243,7 @@
         <v>x66</v>
       </c>
       <c r="C109" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E109" s="38" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
fir filter for surface data
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\firmware-phased-array\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4E3279-4343-41DE-A41F-9AEA3829404E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8F357-5D40-4A68-A887-0573286EE42D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1214,7 +1214,7 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="14" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="82.85546875" customWidth="1"/>
+    <col min="4" max="4" width="87.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
move surface event-select register
</commit_message>
<xml_diff>
--- a/doc/firmware-register-map.xlsx
+++ b/doc/firmware-register-map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Desktop\projects\firmware-phased-array\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8F357-5D40-4A68-A887-0573286EE42D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389A5CA6-D600-49C7-82DA-19B15FB2F398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -680,9 +680,6 @@
     <t>0x380914</t>
   </si>
   <si>
-    <t>0x010002</t>
-  </si>
-  <si>
     <t>lower four bits clear each of the 4 event buffers, bit 8 sets buffer to 0, bit 16 is buffer clear for surface event buffer</t>
   </si>
   <si>
@@ -707,7 +704,10 @@
     <t>Hpol Surface Power threshold</t>
   </si>
   <si>
-    <t>bits(2-0) = min number channels, bit 3 FIR high pass enable, bit 4=require Hpol&gt;Vpol, bit 5 bit 8 = select surface readout, bit 16 enable surface ADCs and surface trigger</t>
+    <t>bits(2-0) = min number channels, bit 3 FIR high pass enable, bit 4=require Hpol&gt;Vpol; bit 8 = select surface readout; bit 16 enable surface ADCs and surface trigger</t>
+  </si>
+  <si>
+    <t>0x01000A</t>
   </si>
 </sst>
 </file>
@@ -1205,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1425,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2212,10 +2212,10 @@
         <v>213</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54" t="s">
         <v>225</v>
-      </c>
-      <c r="E54" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2564,13 +2564,13 @@
         <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2731,13 +2731,13 @@
         <v>69</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E83" t="s">
         <v>218</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2753,7 +2753,7 @@
         <v>143</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -3243,7 +3243,7 @@
         <v>x66</v>
       </c>
       <c r="C109" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E109" s="38" t="s">
         <v>64</v>

</xml_diff>